<commit_message>
Cleaned up code and data when importing from website, still working on displaying chords at tempo and next steps to include playing song in background
</commit_message>
<xml_diff>
--- a/chords.xlsx
+++ b/chords.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B566"/>
+  <dimension ref="A1:B414"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -367,8 +367,10 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="n">
-        <v>0</v>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Chords</t>
+        </is>
       </c>
     </row>
     <row r="2">
@@ -4498,1526 +4500,6 @@
       <c r="B414" t="inlineStr">
         <is>
           <t>Fs_min</t>
-        </is>
-      </c>
-    </row>
-    <row r="415">
-      <c r="A415" s="1" t="n">
-        <v>413</v>
-      </c>
-      <c r="B415" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="416">
-      <c r="A416" s="1" t="n">
-        <v>414</v>
-      </c>
-      <c r="B416" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="417">
-      <c r="A417" s="1" t="n">
-        <v>415</v>
-      </c>
-      <c r="B417" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="418">
-      <c r="A418" s="1" t="n">
-        <v>416</v>
-      </c>
-      <c r="B418" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="419">
-      <c r="A419" s="1" t="n">
-        <v>417</v>
-      </c>
-      <c r="B419" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="420">
-      <c r="A420" s="1" t="n">
-        <v>418</v>
-      </c>
-      <c r="B420" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="421">
-      <c r="A421" s="1" t="n">
-        <v>419</v>
-      </c>
-      <c r="B421" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="422">
-      <c r="A422" s="1" t="n">
-        <v>420</v>
-      </c>
-      <c r="B422" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="423">
-      <c r="A423" s="1" t="n">
-        <v>421</v>
-      </c>
-      <c r="B423" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="424">
-      <c r="A424" s="1" t="n">
-        <v>422</v>
-      </c>
-      <c r="B424" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="425">
-      <c r="A425" s="1" t="n">
-        <v>423</v>
-      </c>
-      <c r="B425" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="426">
-      <c r="A426" s="1" t="n">
-        <v>424</v>
-      </c>
-      <c r="B426" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="427">
-      <c r="A427" s="1" t="n">
-        <v>425</v>
-      </c>
-      <c r="B427" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="428">
-      <c r="A428" s="1" t="n">
-        <v>426</v>
-      </c>
-      <c r="B428" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="429">
-      <c r="A429" s="1" t="n">
-        <v>427</v>
-      </c>
-      <c r="B429" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="430">
-      <c r="A430" s="1" t="n">
-        <v>428</v>
-      </c>
-      <c r="B430" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="431">
-      <c r="A431" s="1" t="n">
-        <v>429</v>
-      </c>
-      <c r="B431" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="432">
-      <c r="A432" s="1" t="n">
-        <v>430</v>
-      </c>
-      <c r="B432" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="433">
-      <c r="A433" s="1" t="n">
-        <v>431</v>
-      </c>
-      <c r="B433" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="434">
-      <c r="A434" s="1" t="n">
-        <v>432</v>
-      </c>
-      <c r="B434" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="435">
-      <c r="A435" s="1" t="n">
-        <v>433</v>
-      </c>
-      <c r="B435" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="436">
-      <c r="A436" s="1" t="n">
-        <v>434</v>
-      </c>
-      <c r="B436" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="437">
-      <c r="A437" s="1" t="n">
-        <v>435</v>
-      </c>
-      <c r="B437" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="438">
-      <c r="A438" s="1" t="n">
-        <v>436</v>
-      </c>
-      <c r="B438" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="439">
-      <c r="A439" s="1" t="n">
-        <v>437</v>
-      </c>
-      <c r="B439" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="440">
-      <c r="A440" s="1" t="n">
-        <v>438</v>
-      </c>
-      <c r="B440" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="441">
-      <c r="A441" s="1" t="n">
-        <v>439</v>
-      </c>
-      <c r="B441" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="442">
-      <c r="A442" s="1" t="n">
-        <v>440</v>
-      </c>
-      <c r="B442" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="443">
-      <c r="A443" s="1" t="n">
-        <v>441</v>
-      </c>
-      <c r="B443" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="444">
-      <c r="A444" s="1" t="n">
-        <v>442</v>
-      </c>
-      <c r="B444" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="445">
-      <c r="A445" s="1" t="n">
-        <v>443</v>
-      </c>
-      <c r="B445" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="446">
-      <c r="A446" s="1" t="n">
-        <v>444</v>
-      </c>
-      <c r="B446" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="447">
-      <c r="A447" s="1" t="n">
-        <v>445</v>
-      </c>
-      <c r="B447" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="448">
-      <c r="A448" s="1" t="n">
-        <v>446</v>
-      </c>
-      <c r="B448" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="449">
-      <c r="A449" s="1" t="n">
-        <v>447</v>
-      </c>
-      <c r="B449" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="450">
-      <c r="A450" s="1" t="n">
-        <v>448</v>
-      </c>
-      <c r="B450" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="451">
-      <c r="A451" s="1" t="n">
-        <v>449</v>
-      </c>
-      <c r="B451" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="452">
-      <c r="A452" s="1" t="n">
-        <v>450</v>
-      </c>
-      <c r="B452" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="453">
-      <c r="A453" s="1" t="n">
-        <v>451</v>
-      </c>
-      <c r="B453" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="454">
-      <c r="A454" s="1" t="n">
-        <v>452</v>
-      </c>
-      <c r="B454" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="455">
-      <c r="A455" s="1" t="n">
-        <v>453</v>
-      </c>
-      <c r="B455" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="456">
-      <c r="A456" s="1" t="n">
-        <v>454</v>
-      </c>
-      <c r="B456" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="457">
-      <c r="A457" s="1" t="n">
-        <v>455</v>
-      </c>
-      <c r="B457" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="458">
-      <c r="A458" s="1" t="n">
-        <v>456</v>
-      </c>
-      <c r="B458" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="459">
-      <c r="A459" s="1" t="n">
-        <v>457</v>
-      </c>
-      <c r="B459" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="460">
-      <c r="A460" s="1" t="n">
-        <v>458</v>
-      </c>
-      <c r="B460" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="461">
-      <c r="A461" s="1" t="n">
-        <v>459</v>
-      </c>
-      <c r="B461" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="462">
-      <c r="A462" s="1" t="n">
-        <v>460</v>
-      </c>
-      <c r="B462" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="463">
-      <c r="A463" s="1" t="n">
-        <v>461</v>
-      </c>
-      <c r="B463" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="464">
-      <c r="A464" s="1" t="n">
-        <v>462</v>
-      </c>
-      <c r="B464" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="465">
-      <c r="A465" s="1" t="n">
-        <v>463</v>
-      </c>
-      <c r="B465" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="466">
-      <c r="A466" s="1" t="n">
-        <v>464</v>
-      </c>
-      <c r="B466" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="467">
-      <c r="A467" s="1" t="n">
-        <v>465</v>
-      </c>
-      <c r="B467" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="468">
-      <c r="A468" s="1" t="n">
-        <v>466</v>
-      </c>
-      <c r="B468" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="469">
-      <c r="A469" s="1" t="n">
-        <v>467</v>
-      </c>
-      <c r="B469" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="470">
-      <c r="A470" s="1" t="n">
-        <v>468</v>
-      </c>
-      <c r="B470" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="471">
-      <c r="A471" s="1" t="n">
-        <v>469</v>
-      </c>
-      <c r="B471" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="472">
-      <c r="A472" s="1" t="n">
-        <v>470</v>
-      </c>
-      <c r="B472" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="473">
-      <c r="A473" s="1" t="n">
-        <v>471</v>
-      </c>
-      <c r="B473" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="474">
-      <c r="A474" s="1" t="n">
-        <v>472</v>
-      </c>
-      <c r="B474" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="475">
-      <c r="A475" s="1" t="n">
-        <v>473</v>
-      </c>
-      <c r="B475" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="476">
-      <c r="A476" s="1" t="n">
-        <v>474</v>
-      </c>
-      <c r="B476" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="477">
-      <c r="A477" s="1" t="n">
-        <v>475</v>
-      </c>
-      <c r="B477" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="478">
-      <c r="A478" s="1" t="n">
-        <v>476</v>
-      </c>
-      <c r="B478" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="479">
-      <c r="A479" s="1" t="n">
-        <v>477</v>
-      </c>
-      <c r="B479" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="480">
-      <c r="A480" s="1" t="n">
-        <v>478</v>
-      </c>
-      <c r="B480" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="481">
-      <c r="A481" s="1" t="n">
-        <v>479</v>
-      </c>
-      <c r="B481" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="482">
-      <c r="A482" s="1" t="n">
-        <v>480</v>
-      </c>
-      <c r="B482" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="483">
-      <c r="A483" s="1" t="n">
-        <v>481</v>
-      </c>
-      <c r="B483" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="484">
-      <c r="A484" s="1" t="n">
-        <v>482</v>
-      </c>
-      <c r="B484" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="485">
-      <c r="A485" s="1" t="n">
-        <v>483</v>
-      </c>
-      <c r="B485" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="486">
-      <c r="A486" s="1" t="n">
-        <v>484</v>
-      </c>
-      <c r="B486" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="487">
-      <c r="A487" s="1" t="n">
-        <v>485</v>
-      </c>
-      <c r="B487" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="488">
-      <c r="A488" s="1" t="n">
-        <v>486</v>
-      </c>
-      <c r="B488" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="489">
-      <c r="A489" s="1" t="n">
-        <v>487</v>
-      </c>
-      <c r="B489" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="490">
-      <c r="A490" s="1" t="n">
-        <v>488</v>
-      </c>
-      <c r="B490" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="491">
-      <c r="A491" s="1" t="n">
-        <v>489</v>
-      </c>
-      <c r="B491" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="492">
-      <c r="A492" s="1" t="n">
-        <v>490</v>
-      </c>
-      <c r="B492" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="493">
-      <c r="A493" s="1" t="n">
-        <v>491</v>
-      </c>
-      <c r="B493" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="494">
-      <c r="A494" s="1" t="n">
-        <v>492</v>
-      </c>
-      <c r="B494" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="495">
-      <c r="A495" s="1" t="n">
-        <v>493</v>
-      </c>
-      <c r="B495" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="496">
-      <c r="A496" s="1" t="n">
-        <v>494</v>
-      </c>
-      <c r="B496" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="497">
-      <c r="A497" s="1" t="n">
-        <v>495</v>
-      </c>
-      <c r="B497" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="498">
-      <c r="A498" s="1" t="n">
-        <v>496</v>
-      </c>
-      <c r="B498" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="499">
-      <c r="A499" s="1" t="n">
-        <v>497</v>
-      </c>
-      <c r="B499" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="500">
-      <c r="A500" s="1" t="n">
-        <v>498</v>
-      </c>
-      <c r="B500" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="501">
-      <c r="A501" s="1" t="n">
-        <v>499</v>
-      </c>
-      <c r="B501" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="502">
-      <c r="A502" s="1" t="n">
-        <v>500</v>
-      </c>
-      <c r="B502" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="503">
-      <c r="A503" s="1" t="n">
-        <v>501</v>
-      </c>
-      <c r="B503" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="504">
-      <c r="A504" s="1" t="n">
-        <v>502</v>
-      </c>
-      <c r="B504" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="505">
-      <c r="A505" s="1" t="n">
-        <v>503</v>
-      </c>
-      <c r="B505" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="506">
-      <c r="A506" s="1" t="n">
-        <v>504</v>
-      </c>
-      <c r="B506" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="507">
-      <c r="A507" s="1" t="n">
-        <v>505</v>
-      </c>
-      <c r="B507" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="508">
-      <c r="A508" s="1" t="n">
-        <v>506</v>
-      </c>
-      <c r="B508" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="509">
-      <c r="A509" s="1" t="n">
-        <v>507</v>
-      </c>
-      <c r="B509" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="510">
-      <c r="A510" s="1" t="n">
-        <v>508</v>
-      </c>
-      <c r="B510" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="511">
-      <c r="A511" s="1" t="n">
-        <v>509</v>
-      </c>
-      <c r="B511" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="512">
-      <c r="A512" s="1" t="n">
-        <v>510</v>
-      </c>
-      <c r="B512" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="513">
-      <c r="A513" s="1" t="n">
-        <v>511</v>
-      </c>
-      <c r="B513" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="514">
-      <c r="A514" s="1" t="n">
-        <v>512</v>
-      </c>
-      <c r="B514" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="515">
-      <c r="A515" s="1" t="n">
-        <v>513</v>
-      </c>
-      <c r="B515" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="516">
-      <c r="A516" s="1" t="n">
-        <v>514</v>
-      </c>
-      <c r="B516" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="517">
-      <c r="A517" s="1" t="n">
-        <v>515</v>
-      </c>
-      <c r="B517" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="518">
-      <c r="A518" s="1" t="n">
-        <v>516</v>
-      </c>
-      <c r="B518" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="519">
-      <c r="A519" s="1" t="n">
-        <v>517</v>
-      </c>
-      <c r="B519" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="520">
-      <c r="A520" s="1" t="n">
-        <v>518</v>
-      </c>
-      <c r="B520" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="521">
-      <c r="A521" s="1" t="n">
-        <v>519</v>
-      </c>
-      <c r="B521" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="522">
-      <c r="A522" s="1" t="n">
-        <v>520</v>
-      </c>
-      <c r="B522" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="523">
-      <c r="A523" s="1" t="n">
-        <v>521</v>
-      </c>
-      <c r="B523" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="524">
-      <c r="A524" s="1" t="n">
-        <v>522</v>
-      </c>
-      <c r="B524" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="525">
-      <c r="A525" s="1" t="n">
-        <v>523</v>
-      </c>
-      <c r="B525" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="526">
-      <c r="A526" s="1" t="n">
-        <v>524</v>
-      </c>
-      <c r="B526" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="527">
-      <c r="A527" s="1" t="n">
-        <v>525</v>
-      </c>
-      <c r="B527" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="528">
-      <c r="A528" s="1" t="n">
-        <v>526</v>
-      </c>
-      <c r="B528" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="529">
-      <c r="A529" s="1" t="n">
-        <v>527</v>
-      </c>
-      <c r="B529" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="530">
-      <c r="A530" s="1" t="n">
-        <v>528</v>
-      </c>
-      <c r="B530" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="531">
-      <c r="A531" s="1" t="n">
-        <v>529</v>
-      </c>
-      <c r="B531" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="532">
-      <c r="A532" s="1" t="n">
-        <v>530</v>
-      </c>
-      <c r="B532" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="533">
-      <c r="A533" s="1" t="n">
-        <v>531</v>
-      </c>
-      <c r="B533" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="534">
-      <c r="A534" s="1" t="n">
-        <v>532</v>
-      </c>
-      <c r="B534" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="535">
-      <c r="A535" s="1" t="n">
-        <v>533</v>
-      </c>
-      <c r="B535" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="536">
-      <c r="A536" s="1" t="n">
-        <v>534</v>
-      </c>
-      <c r="B536" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="537">
-      <c r="A537" s="1" t="n">
-        <v>535</v>
-      </c>
-      <c r="B537" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="538">
-      <c r="A538" s="1" t="n">
-        <v>536</v>
-      </c>
-      <c r="B538" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="539">
-      <c r="A539" s="1" t="n">
-        <v>537</v>
-      </c>
-      <c r="B539" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="540">
-      <c r="A540" s="1" t="n">
-        <v>538</v>
-      </c>
-      <c r="B540" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="541">
-      <c r="A541" s="1" t="n">
-        <v>539</v>
-      </c>
-      <c r="B541" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="542">
-      <c r="A542" s="1" t="n">
-        <v>540</v>
-      </c>
-      <c r="B542" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="543">
-      <c r="A543" s="1" t="n">
-        <v>541</v>
-      </c>
-      <c r="B543" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="544">
-      <c r="A544" s="1" t="n">
-        <v>542</v>
-      </c>
-      <c r="B544" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="545">
-      <c r="A545" s="1" t="n">
-        <v>543</v>
-      </c>
-      <c r="B545" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="546">
-      <c r="A546" s="1" t="n">
-        <v>544</v>
-      </c>
-      <c r="B546" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="547">
-      <c r="A547" s="1" t="n">
-        <v>545</v>
-      </c>
-      <c r="B547" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="548">
-      <c r="A548" s="1" t="n">
-        <v>546</v>
-      </c>
-      <c r="B548" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="549">
-      <c r="A549" s="1" t="n">
-        <v>547</v>
-      </c>
-      <c r="B549" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="550">
-      <c r="A550" s="1" t="n">
-        <v>548</v>
-      </c>
-      <c r="B550" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="551">
-      <c r="A551" s="1" t="n">
-        <v>549</v>
-      </c>
-      <c r="B551" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="552">
-      <c r="A552" s="1" t="n">
-        <v>550</v>
-      </c>
-      <c r="B552" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="553">
-      <c r="A553" s="1" t="n">
-        <v>551</v>
-      </c>
-      <c r="B553" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="554">
-      <c r="A554" s="1" t="n">
-        <v>552</v>
-      </c>
-      <c r="B554" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="555">
-      <c r="A555" s="1" t="n">
-        <v>553</v>
-      </c>
-      <c r="B555" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="556">
-      <c r="A556" s="1" t="n">
-        <v>554</v>
-      </c>
-      <c r="B556" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="557">
-      <c r="A557" s="1" t="n">
-        <v>555</v>
-      </c>
-      <c r="B557" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="558">
-      <c r="A558" s="1" t="n">
-        <v>556</v>
-      </c>
-      <c r="B558" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="559">
-      <c r="A559" s="1" t="n">
-        <v>557</v>
-      </c>
-      <c r="B559" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="560">
-      <c r="A560" s="1" t="n">
-        <v>558</v>
-      </c>
-      <c r="B560" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="561">
-      <c r="A561" s="1" t="n">
-        <v>559</v>
-      </c>
-      <c r="B561" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="562">
-      <c r="A562" s="1" t="n">
-        <v>560</v>
-      </c>
-      <c r="B562" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="563">
-      <c r="A563" s="1" t="n">
-        <v>561</v>
-      </c>
-      <c r="B563" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="564">
-      <c r="A564" s="1" t="n">
-        <v>562</v>
-      </c>
-      <c r="B564" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="565">
-      <c r="A565" s="1" t="n">
-        <v>563</v>
-      </c>
-      <c r="B565" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
-        </is>
-      </c>
-    </row>
-    <row r="566">
-      <c r="A566" s="1" t="n">
-        <v>564</v>
-      </c>
-      <c r="B566" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  </t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Formatted and finalized the output tool to dispaly chords to user
</commit_message>
<xml_diff>
--- a/chords.xlsx
+++ b/chords.xlsx
@@ -379,7 +379,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -389,7 +389,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -399,7 +399,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -409,7 +409,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -419,7 +419,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>A_maj</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -429,7 +429,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>A_maj</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -439,7 +439,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -449,7 +449,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -459,7 +459,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -469,7 +469,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -479,7 +479,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -489,7 +489,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -499,7 +499,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>A_7</t>
+          <t>A7</t>
         </is>
       </c>
     </row>
@@ -509,7 +509,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>A_7</t>
+          <t>A7</t>
         </is>
       </c>
     </row>
@@ -519,7 +519,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -529,7 +529,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -539,7 +539,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -549,7 +549,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -559,7 +559,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -569,7 +569,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -579,7 +579,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Fs_7</t>
+          <t>F#7</t>
         </is>
       </c>
     </row>
@@ -589,7 +589,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Fs_7</t>
+          <t>F#7</t>
         </is>
       </c>
     </row>
@@ -599,7 +599,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -609,7 +609,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -619,7 +619,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Fs_min7</t>
+          <t>F#m7</t>
         </is>
       </c>
     </row>
@@ -629,7 +629,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Fs_min7</t>
+          <t>F#m7</t>
         </is>
       </c>
     </row>
@@ -639,7 +639,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Fs_maj</t>
+          <t>F#</t>
         </is>
       </c>
     </row>
@@ -649,7 +649,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Fs_maj</t>
+          <t>F#</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>A_7</t>
+          <t>A7</t>
         </is>
       </c>
     </row>
@@ -669,7 +669,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -679,7 +679,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -689,7 +689,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -699,7 +699,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Fs_min7</t>
+          <t>F#m7</t>
         </is>
       </c>
     </row>
@@ -709,7 +709,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Fs_min7</t>
+          <t>F#m7</t>
         </is>
       </c>
     </row>
@@ -719,7 +719,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Fs_min7</t>
+          <t>F#m7</t>
         </is>
       </c>
     </row>
@@ -729,7 +729,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Fs_min7</t>
+          <t>F#m7</t>
         </is>
       </c>
     </row>
@@ -739,7 +739,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Fs_min7</t>
+          <t>F#m7</t>
         </is>
       </c>
     </row>
@@ -749,7 +749,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Fs_min7</t>
+          <t>F#m7</t>
         </is>
       </c>
     </row>
@@ -759,7 +759,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Fs_min7</t>
+          <t>F#m7</t>
         </is>
       </c>
     </row>
@@ -769,7 +769,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Fs_min7</t>
+          <t>F#m7</t>
         </is>
       </c>
     </row>
@@ -779,7 +779,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Fs_maj</t>
+          <t>F#</t>
         </is>
       </c>
     </row>
@@ -789,7 +789,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Fs_maj</t>
+          <t>F#</t>
         </is>
       </c>
     </row>
@@ -799,7 +799,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Fs_maj</t>
+          <t>F#</t>
         </is>
       </c>
     </row>
@@ -809,7 +809,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Fs_maj</t>
+          <t>F#</t>
         </is>
       </c>
     </row>
@@ -819,7 +819,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>A_maj</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -829,7 +829,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>A_maj</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -839,7 +839,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -849,7 +849,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -859,7 +859,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -869,7 +869,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -879,7 +879,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -889,7 +889,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -899,7 +899,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>A_maj</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -909,7 +909,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>A_maj</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -919,7 +919,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -929,7 +929,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -939,7 +939,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -949,7 +949,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -959,7 +959,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Fs_maj</t>
+          <t>F#</t>
         </is>
       </c>
     </row>
@@ -969,7 +969,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Fs_maj</t>
+          <t>F#</t>
         </is>
       </c>
     </row>
@@ -979,7 +979,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>A_maj</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -989,7 +989,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -999,7 +999,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -1009,7 +1009,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -1019,7 +1019,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -1029,7 +1029,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -1039,7 +1039,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -1049,7 +1049,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -1059,7 +1059,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>A_maj</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -1069,7 +1069,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -1079,7 +1079,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -1089,7 +1089,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -1099,7 +1099,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -1109,7 +1109,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -1119,7 +1119,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -1129,7 +1129,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -1139,7 +1139,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>A_maj</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -1149,7 +1149,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>A_maj</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -1159,7 +1159,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -1169,7 +1169,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -1179,7 +1179,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -1189,7 +1189,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -1199,7 +1199,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>A_maj</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -1209,7 +1209,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>A_maj</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -1219,7 +1219,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>A_7</t>
+          <t>A7</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>A_7</t>
+          <t>A7</t>
         </is>
       </c>
     </row>
@@ -1239,7 +1239,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>A_7</t>
+          <t>A7</t>
         </is>
       </c>
     </row>
@@ -1249,7 +1249,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>A_7</t>
+          <t>A7</t>
         </is>
       </c>
     </row>
@@ -1259,7 +1259,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -1269,7 +1269,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -1279,7 +1279,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -1289,7 +1289,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -1299,7 +1299,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>A_7</t>
+          <t>A7</t>
         </is>
       </c>
     </row>
@@ -1309,7 +1309,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -1319,7 +1319,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -1329,7 +1329,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -1339,7 +1339,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -1349,7 +1349,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -1359,7 +1359,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -1369,7 +1369,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -1379,7 +1379,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>A_7</t>
+          <t>A7</t>
         </is>
       </c>
     </row>
@@ -1389,7 +1389,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -1399,7 +1399,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -1409,7 +1409,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -1419,7 +1419,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -1429,7 +1429,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -1439,7 +1439,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>D_maj</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -1449,7 +1449,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>D_maj</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -1459,7 +1459,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>A_maj</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -1469,7 +1469,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -1479,7 +1479,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -1489,7 +1489,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -1499,7 +1499,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Fs_min7</t>
+          <t>F#m7</t>
         </is>
       </c>
     </row>
@@ -1509,7 +1509,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Fs_min7</t>
+          <t>F#m7</t>
         </is>
       </c>
     </row>
@@ -1519,7 +1519,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Fs_maj</t>
+          <t>F#</t>
         </is>
       </c>
     </row>
@@ -1529,7 +1529,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Fs_maj</t>
+          <t>F#</t>
         </is>
       </c>
     </row>
@@ -1539,7 +1539,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>A_maj</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -1549,7 +1549,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -1559,7 +1559,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -1569,7 +1569,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -1579,7 +1579,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -1589,7 +1589,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -1599,7 +1599,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -1609,7 +1609,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>A_maj</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -1619,7 +1619,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>A_7</t>
+          <t>A7</t>
         </is>
       </c>
     </row>
@@ -1629,7 +1629,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>A_7</t>
+          <t>A7</t>
         </is>
       </c>
     </row>
@@ -1639,7 +1639,7 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -1649,7 +1649,7 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -1659,7 +1659,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>D_7</t>
+          <t>D7</t>
         </is>
       </c>
     </row>
@@ -1669,7 +1669,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>D_7</t>
+          <t>D7</t>
         </is>
       </c>
     </row>
@@ -1679,7 +1679,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -1689,7 +1689,7 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -1699,7 +1699,7 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>Fs_min7</t>
+          <t>F#m7</t>
         </is>
       </c>
     </row>
@@ -1709,7 +1709,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>Fs_min7</t>
+          <t>F#m7</t>
         </is>
       </c>
     </row>
@@ -1719,7 +1719,7 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>Fs_min7</t>
+          <t>F#m7</t>
         </is>
       </c>
     </row>
@@ -1729,7 +1729,7 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Fs_min7</t>
+          <t>F#m7</t>
         </is>
       </c>
     </row>
@@ -1739,7 +1739,7 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>D_7</t>
+          <t>D7</t>
         </is>
       </c>
     </row>
@@ -1749,7 +1749,7 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -1759,7 +1759,7 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -1769,7 +1769,7 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -1779,7 +1779,7 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>Fs_min7</t>
+          <t>F#m7</t>
         </is>
       </c>
     </row>
@@ -1789,7 +1789,7 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>Fs_min7</t>
+          <t>F#m7</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>Fs_min7</t>
+          <t>F#m7</t>
         </is>
       </c>
     </row>
@@ -1809,7 +1809,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>Fs_min7</t>
+          <t>F#m7</t>
         </is>
       </c>
     </row>
@@ -1819,7 +1819,7 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>D_7</t>
+          <t>D7</t>
         </is>
       </c>
     </row>
@@ -1829,7 +1829,7 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -1839,7 +1839,7 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -1849,7 +1849,7 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -1859,7 +1859,7 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>Fs_min7</t>
+          <t>F#m7</t>
         </is>
       </c>
     </row>
@@ -1869,7 +1869,7 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>Fs_min7</t>
+          <t>F#m7</t>
         </is>
       </c>
     </row>
@@ -1879,7 +1879,7 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>Fs_min7</t>
+          <t>F#m7</t>
         </is>
       </c>
     </row>
@@ -1889,7 +1889,7 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>Fs_min7</t>
+          <t>F#m7</t>
         </is>
       </c>
     </row>
@@ -1899,7 +1899,7 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>Gs_7</t>
+          <t>G#7</t>
         </is>
       </c>
     </row>
@@ -1909,7 +1909,7 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>Gs_7</t>
+          <t>G#7</t>
         </is>
       </c>
     </row>
@@ -1919,7 +1919,7 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>Gs_7</t>
+          <t>G#7</t>
         </is>
       </c>
     </row>
@@ -1929,7 +1929,7 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>Gs_7</t>
+          <t>G#7</t>
         </is>
       </c>
     </row>
@@ -1939,7 +1939,7 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -1949,7 +1949,7 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -1959,7 +1959,7 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -1969,7 +1969,7 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -1979,7 +1979,7 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -1989,7 +1989,7 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -1999,7 +1999,7 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -2009,7 +2009,7 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -2019,7 +2019,7 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>Fs_maj</t>
+          <t>F#</t>
         </is>
       </c>
     </row>
@@ -2029,7 +2029,7 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>Fs_maj</t>
+          <t>F#</t>
         </is>
       </c>
     </row>
@@ -2039,7 +2039,7 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -2049,7 +2049,7 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -2059,7 +2059,7 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>Fs_maj</t>
+          <t>F#</t>
         </is>
       </c>
     </row>
@@ -2069,7 +2069,7 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Fs_maj</t>
+          <t>F#</t>
         </is>
       </c>
     </row>
@@ -2079,7 +2079,7 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>Fs_maj</t>
+          <t>F#</t>
         </is>
       </c>
     </row>
@@ -2089,7 +2089,7 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>Fs_maj</t>
+          <t>F#</t>
         </is>
       </c>
     </row>
@@ -2099,7 +2099,7 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>A_7</t>
+          <t>A7</t>
         </is>
       </c>
     </row>
@@ -2109,7 +2109,7 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -2119,7 +2119,7 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -2129,7 +2129,7 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -2139,7 +2139,7 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -2149,7 +2149,7 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -2159,7 +2159,7 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>D_maj</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -2169,7 +2169,7 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>D_maj</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -2179,7 +2179,7 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>A_7</t>
+          <t>A7</t>
         </is>
       </c>
     </row>
@@ -2189,7 +2189,7 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>A_7</t>
+          <t>A7</t>
         </is>
       </c>
     </row>
@@ -2199,7 +2199,7 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>A_7</t>
+          <t>A7</t>
         </is>
       </c>
     </row>
@@ -2209,7 +2209,7 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>A_7</t>
+          <t>A7</t>
         </is>
       </c>
     </row>
@@ -2219,7 +2219,7 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -2229,7 +2229,7 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -2239,7 +2239,7 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>A_maj</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -2249,7 +2249,7 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>A_maj</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -2259,7 +2259,7 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>A_7</t>
+          <t>A7</t>
         </is>
       </c>
     </row>
@@ -2269,7 +2269,7 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -2279,7 +2279,7 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -2289,7 +2289,7 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -2299,7 +2299,7 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -2309,7 +2309,7 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -2319,7 +2319,7 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>D_maj</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -2329,7 +2329,7 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>D_maj</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -2339,7 +2339,7 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>A_7</t>
+          <t>A7</t>
         </is>
       </c>
     </row>
@@ -2349,7 +2349,7 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>A_7</t>
+          <t>A7</t>
         </is>
       </c>
     </row>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -2379,7 +2379,7 @@
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -2389,7 +2389,7 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -2399,7 +2399,7 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -2409,7 +2409,7 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -2419,7 +2419,7 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>A_7</t>
+          <t>A7</t>
         </is>
       </c>
     </row>
@@ -2429,7 +2429,7 @@
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>A_7</t>
+          <t>A7</t>
         </is>
       </c>
     </row>
@@ -2439,7 +2439,7 @@
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -2449,7 +2449,7 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -2459,7 +2459,7 @@
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -2469,7 +2469,7 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -2479,7 +2479,7 @@
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -2489,7 +2489,7 @@
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -2499,7 +2499,7 @@
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>A_maj</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -2509,7 +2509,7 @@
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>A_maj</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -2519,7 +2519,7 @@
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>A_maj</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -2529,7 +2529,7 @@
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>A_maj</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -2539,7 +2539,7 @@
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -2549,7 +2549,7 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -2559,7 +2559,7 @@
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -2569,7 +2569,7 @@
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -2579,7 +2579,7 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>A_7</t>
+          <t>A7</t>
         </is>
       </c>
     </row>
@@ -2589,7 +2589,7 @@
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>A_7</t>
+          <t>A7</t>
         </is>
       </c>
     </row>
@@ -2599,7 +2599,7 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>A_7</t>
+          <t>A7</t>
         </is>
       </c>
     </row>
@@ -2609,7 +2609,7 @@
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>A_7</t>
+          <t>A7</t>
         </is>
       </c>
     </row>
@@ -2619,7 +2619,7 @@
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -2629,7 +2629,7 @@
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -2639,7 +2639,7 @@
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>D_maj</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -2649,7 +2649,7 @@
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>D_maj</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -2659,7 +2659,7 @@
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>A_maj</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -2669,7 +2669,7 @@
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>A_maj</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -2679,7 +2679,7 @@
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>A_maj</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -2689,7 +2689,7 @@
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>A_maj</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -2699,7 +2699,7 @@
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -2709,7 +2709,7 @@
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -2719,7 +2719,7 @@
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>D_maj</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -2729,7 +2729,7 @@
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>D_maj</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -2739,7 +2739,7 @@
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>A_maj</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -2749,7 +2749,7 @@
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -2759,7 +2759,7 @@
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -2769,7 +2769,7 @@
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -2779,7 +2779,7 @@
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -2789,7 +2789,7 @@
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -2799,7 +2799,7 @@
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>D_maj</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -2809,7 +2809,7 @@
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>D_maj</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -2819,7 +2819,7 @@
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>A_maj</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -2829,7 +2829,7 @@
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -2839,7 +2839,7 @@
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -2849,7 +2849,7 @@
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -2859,7 +2859,7 @@
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -2869,7 +2869,7 @@
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -2879,7 +2879,7 @@
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>A_7</t>
+          <t>A7</t>
         </is>
       </c>
     </row>
@@ -2889,7 +2889,7 @@
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>A_7</t>
+          <t>A7</t>
         </is>
       </c>
     </row>
@@ -2899,7 +2899,7 @@
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>A_7</t>
+          <t>A7</t>
         </is>
       </c>
     </row>
@@ -2909,7 +2909,7 @@
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>A_7</t>
+          <t>A7</t>
         </is>
       </c>
     </row>
@@ -2919,7 +2919,7 @@
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -2929,7 +2929,7 @@
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -2939,7 +2939,7 @@
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>D_maj</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -2949,7 +2949,7 @@
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>D_maj</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -2959,7 +2959,7 @@
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>D_7</t>
+          <t>D7</t>
         </is>
       </c>
     </row>
@@ -2969,7 +2969,7 @@
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>D_7</t>
+          <t>D7</t>
         </is>
       </c>
     </row>
@@ -2979,7 +2979,7 @@
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>Fs_7</t>
+          <t>F#7</t>
         </is>
       </c>
     </row>
@@ -2989,7 +2989,7 @@
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>Fs_7</t>
+          <t>F#7</t>
         </is>
       </c>
     </row>
@@ -2999,7 +2999,7 @@
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>Fs_7</t>
+          <t>F#7</t>
         </is>
       </c>
     </row>
@@ -3009,7 +3009,7 @@
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>Fs_7</t>
+          <t>F#7</t>
         </is>
       </c>
     </row>
@@ -3019,7 +3019,7 @@
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>D_maj</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -3029,7 +3029,7 @@
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>D_maj</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -3039,7 +3039,7 @@
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -3049,7 +3049,7 @@
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -3059,7 +3059,7 @@
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>Fs_min7</t>
+          <t>F#m7</t>
         </is>
       </c>
     </row>
@@ -3069,7 +3069,7 @@
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>Fs_min7</t>
+          <t>F#m7</t>
         </is>
       </c>
     </row>
@@ -3079,7 +3079,7 @@
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>Fs_min7</t>
+          <t>F#m7</t>
         </is>
       </c>
     </row>
@@ -3089,7 +3089,7 @@
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>Fs_min7</t>
+          <t>F#m7</t>
         </is>
       </c>
     </row>
@@ -3099,7 +3099,7 @@
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>D_maj</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -3109,7 +3109,7 @@
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>D_maj</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -3119,7 +3119,7 @@
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -3129,7 +3129,7 @@
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -3139,7 +3139,7 @@
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>Fs_min7</t>
+          <t>F#m7</t>
         </is>
       </c>
     </row>
@@ -3149,7 +3149,7 @@
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>Fs_min7</t>
+          <t>F#m7</t>
         </is>
       </c>
     </row>
@@ -3159,7 +3159,7 @@
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>Fs_min7</t>
+          <t>F#m7</t>
         </is>
       </c>
     </row>
@@ -3169,7 +3169,7 @@
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>Fs_min7</t>
+          <t>F#m7</t>
         </is>
       </c>
     </row>
@@ -3179,7 +3179,7 @@
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>Gs_7</t>
+          <t>G#7</t>
         </is>
       </c>
     </row>
@@ -3189,7 +3189,7 @@
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>Gs_7</t>
+          <t>G#7</t>
         </is>
       </c>
     </row>
@@ -3199,7 +3199,7 @@
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>Gs_7</t>
+          <t>G#7</t>
         </is>
       </c>
     </row>
@@ -3209,7 +3209,7 @@
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>Gs_7</t>
+          <t>G#7</t>
         </is>
       </c>
     </row>
@@ -3219,7 +3219,7 @@
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -3229,7 +3229,7 @@
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -3239,7 +3239,7 @@
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -3249,7 +3249,7 @@
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -3259,7 +3259,7 @@
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>Fs_min7</t>
+          <t>F#m7</t>
         </is>
       </c>
     </row>
@@ -3269,7 +3269,7 @@
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>Fs_min7</t>
+          <t>F#m7</t>
         </is>
       </c>
     </row>
@@ -3279,7 +3279,7 @@
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>Fs_min7</t>
+          <t>F#m7</t>
         </is>
       </c>
     </row>
@@ -3289,7 +3289,7 @@
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>Fs_min7</t>
+          <t>F#m7</t>
         </is>
       </c>
     </row>
@@ -3299,7 +3299,7 @@
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>A_7</t>
+          <t>A7</t>
         </is>
       </c>
     </row>
@@ -3309,7 +3309,7 @@
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>A_7</t>
+          <t>A7</t>
         </is>
       </c>
     </row>
@@ -3319,7 +3319,7 @@
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>A_7</t>
+          <t>A7</t>
         </is>
       </c>
     </row>
@@ -3329,7 +3329,7 @@
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>A_7</t>
+          <t>A7</t>
         </is>
       </c>
     </row>
@@ -3339,7 +3339,7 @@
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>Fs_min7</t>
+          <t>F#m7</t>
         </is>
       </c>
     </row>
@@ -3349,7 +3349,7 @@
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>Fs_min7</t>
+          <t>F#m7</t>
         </is>
       </c>
     </row>
@@ -3359,7 +3359,7 @@
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>D_maj</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -3369,7 +3369,7 @@
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>D_maj</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -3379,7 +3379,7 @@
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>A_7</t>
+          <t>A7</t>
         </is>
       </c>
     </row>
@@ -3389,7 +3389,7 @@
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>A_7</t>
+          <t>A7</t>
         </is>
       </c>
     </row>
@@ -3399,7 +3399,7 @@
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -3409,7 +3409,7 @@
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -3419,7 +3419,7 @@
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -3429,7 +3429,7 @@
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -3439,7 +3439,7 @@
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -3449,7 +3449,7 @@
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -3459,7 +3459,7 @@
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>A_7</t>
+          <t>A7</t>
         </is>
       </c>
     </row>
@@ -3469,7 +3469,7 @@
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>A_7</t>
+          <t>A7</t>
         </is>
       </c>
     </row>
@@ -3479,7 +3479,7 @@
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -3489,7 +3489,7 @@
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -3499,7 +3499,7 @@
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -3509,7 +3509,7 @@
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -3519,7 +3519,7 @@
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -3529,7 +3529,7 @@
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>A_maj</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -3539,7 +3539,7 @@
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>A_7</t>
+          <t>A7</t>
         </is>
       </c>
     </row>
@@ -3549,7 +3549,7 @@
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>A_7</t>
+          <t>A7</t>
         </is>
       </c>
     </row>
@@ -3559,7 +3559,7 @@
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>A_7</t>
+          <t>A7</t>
         </is>
       </c>
     </row>
@@ -3569,7 +3569,7 @@
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>A_7</t>
+          <t>A7</t>
         </is>
       </c>
     </row>
@@ -3579,7 +3579,7 @@
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -3589,7 +3589,7 @@
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -3599,7 +3599,7 @@
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -3609,7 +3609,7 @@
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -3619,7 +3619,7 @@
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>A_maj</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -3629,7 +3629,7 @@
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>A_maj</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -3639,7 +3639,7 @@
       </c>
       <c r="B328" t="inlineStr">
         <is>
-          <t>A_maj</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -3649,7 +3649,7 @@
       </c>
       <c r="B329" t="inlineStr">
         <is>
-          <t>A_maj</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -3659,7 +3659,7 @@
       </c>
       <c r="B330" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -3669,7 +3669,7 @@
       </c>
       <c r="B331" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -3679,7 +3679,7 @@
       </c>
       <c r="B332" t="inlineStr">
         <is>
-          <t>D_maj</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -3689,7 +3689,7 @@
       </c>
       <c r="B333" t="inlineStr">
         <is>
-          <t>D_maj</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -3699,7 +3699,7 @@
       </c>
       <c r="B334" t="inlineStr">
         <is>
-          <t>A_maj</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -3709,7 +3709,7 @@
       </c>
       <c r="B335" t="inlineStr">
         <is>
-          <t>A_maj</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -3719,7 +3719,7 @@
       </c>
       <c r="B336" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -3729,7 +3729,7 @@
       </c>
       <c r="B337" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -3739,7 +3739,7 @@
       </c>
       <c r="B338" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -3749,7 +3749,7 @@
       </c>
       <c r="B339" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -3759,7 +3759,7 @@
       </c>
       <c r="B340" t="inlineStr">
         <is>
-          <t>D_maj</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -3769,7 +3769,7 @@
       </c>
       <c r="B341" t="inlineStr">
         <is>
-          <t>D_maj</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -3779,7 +3779,7 @@
       </c>
       <c r="B342" t="inlineStr">
         <is>
-          <t>A_maj</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -3789,7 +3789,7 @@
       </c>
       <c r="B343" t="inlineStr">
         <is>
-          <t>A_maj</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -3799,7 +3799,7 @@
       </c>
       <c r="B344" t="inlineStr">
         <is>
-          <t>A_maj</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -3809,7 +3809,7 @@
       </c>
       <c r="B345" t="inlineStr">
         <is>
-          <t>A_maj</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -3819,7 +3819,7 @@
       </c>
       <c r="B346" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -3829,7 +3829,7 @@
       </c>
       <c r="B347" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -3839,7 +3839,7 @@
       </c>
       <c r="B348" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -3849,7 +3849,7 @@
       </c>
       <c r="B349" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -3859,7 +3859,7 @@
       </c>
       <c r="B350" t="inlineStr">
         <is>
-          <t>A_maj</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -3869,7 +3869,7 @@
       </c>
       <c r="B351" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -3879,7 +3879,7 @@
       </c>
       <c r="B352" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -3889,7 +3889,7 @@
       </c>
       <c r="B353" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -3899,7 +3899,7 @@
       </c>
       <c r="B354" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -3909,7 +3909,7 @@
       </c>
       <c r="B355" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -3919,7 +3919,7 @@
       </c>
       <c r="B356" t="inlineStr">
         <is>
-          <t>D_maj</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -3929,7 +3929,7 @@
       </c>
       <c r="B357" t="inlineStr">
         <is>
-          <t>D_maj</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -3939,7 +3939,7 @@
       </c>
       <c r="B358" t="inlineStr">
         <is>
-          <t>A_7</t>
+          <t>A7</t>
         </is>
       </c>
     </row>
@@ -3949,7 +3949,7 @@
       </c>
       <c r="B359" t="inlineStr">
         <is>
-          <t>A_7</t>
+          <t>A7</t>
         </is>
       </c>
     </row>
@@ -3959,7 +3959,7 @@
       </c>
       <c r="B360" t="inlineStr">
         <is>
-          <t>A_7</t>
+          <t>A7</t>
         </is>
       </c>
     </row>
@@ -3969,7 +3969,7 @@
       </c>
       <c r="B361" t="inlineStr">
         <is>
-          <t>A_7</t>
+          <t>A7</t>
         </is>
       </c>
     </row>
@@ -3979,7 +3979,7 @@
       </c>
       <c r="B362" t="inlineStr">
         <is>
-          <t>Fs_min7</t>
+          <t>F#m7</t>
         </is>
       </c>
     </row>
@@ -3989,7 +3989,7 @@
       </c>
       <c r="B363" t="inlineStr">
         <is>
-          <t>Fs_min7</t>
+          <t>F#m7</t>
         </is>
       </c>
     </row>
@@ -3999,7 +3999,7 @@
       </c>
       <c r="B364" t="inlineStr">
         <is>
-          <t>D_maj</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -4009,7 +4009,7 @@
       </c>
       <c r="B365" t="inlineStr">
         <is>
-          <t>D_maj</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -4019,7 +4019,7 @@
       </c>
       <c r="B366" t="inlineStr">
         <is>
-          <t>A_7</t>
+          <t>A7</t>
         </is>
       </c>
     </row>
@@ -4029,7 +4029,7 @@
       </c>
       <c r="B367" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -4039,7 +4039,7 @@
       </c>
       <c r="B368" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -4049,7 +4049,7 @@
       </c>
       <c r="B369" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -4059,7 +4059,7 @@
       </c>
       <c r="B370" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -4069,7 +4069,7 @@
       </c>
       <c r="B371" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -4079,7 +4079,7 @@
       </c>
       <c r="B372" t="inlineStr">
         <is>
-          <t>D_maj</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -4089,7 +4089,7 @@
       </c>
       <c r="B373" t="inlineStr">
         <is>
-          <t>D_maj</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -4099,7 +4099,7 @@
       </c>
       <c r="B374" t="inlineStr">
         <is>
-          <t>A_7</t>
+          <t>A7</t>
         </is>
       </c>
     </row>
@@ -4109,7 +4109,7 @@
       </c>
       <c r="B375" t="inlineStr">
         <is>
-          <t>A_7</t>
+          <t>A7</t>
         </is>
       </c>
     </row>
@@ -4119,7 +4119,7 @@
       </c>
       <c r="B376" t="inlineStr">
         <is>
-          <t>A_7</t>
+          <t>A7</t>
         </is>
       </c>
     </row>
@@ -4129,7 +4129,7 @@
       </c>
       <c r="B377" t="inlineStr">
         <is>
-          <t>A_7</t>
+          <t>A7</t>
         </is>
       </c>
     </row>
@@ -4139,7 +4139,7 @@
       </c>
       <c r="B378" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -4149,7 +4149,7 @@
       </c>
       <c r="B379" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -4159,7 +4159,7 @@
       </c>
       <c r="B380" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -4169,7 +4169,7 @@
       </c>
       <c r="B381" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -4179,7 +4179,7 @@
       </c>
       <c r="B382" t="inlineStr">
         <is>
-          <t>A_7</t>
+          <t>A7</t>
         </is>
       </c>
     </row>
@@ -4189,7 +4189,7 @@
       </c>
       <c r="B383" t="inlineStr">
         <is>
-          <t>A_7</t>
+          <t>A7</t>
         </is>
       </c>
     </row>
@@ -4199,7 +4199,7 @@
       </c>
       <c r="B384" t="inlineStr">
         <is>
-          <t>A_7</t>
+          <t>A7</t>
         </is>
       </c>
     </row>
@@ -4209,7 +4209,7 @@
       </c>
       <c r="B385" t="inlineStr">
         <is>
-          <t>A_7</t>
+          <t>A7</t>
         </is>
       </c>
     </row>
@@ -4219,7 +4219,7 @@
       </c>
       <c r="B386" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -4229,7 +4229,7 @@
       </c>
       <c r="B387" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -4239,7 +4239,7 @@
       </c>
       <c r="B388" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -4249,7 +4249,7 @@
       </c>
       <c r="B389" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -4259,7 +4259,7 @@
       </c>
       <c r="B390" t="inlineStr">
         <is>
-          <t>A_maj</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -4269,7 +4269,7 @@
       </c>
       <c r="B391" t="inlineStr">
         <is>
-          <t>A_maj</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -4279,7 +4279,7 @@
       </c>
       <c r="B392" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -4289,7 +4289,7 @@
       </c>
       <c r="B393" t="inlineStr">
         <is>
-          <t>Cs_7</t>
+          <t>C#7</t>
         </is>
       </c>
     </row>
@@ -4299,7 +4299,7 @@
       </c>
       <c r="B394" t="inlineStr">
         <is>
-          <t>Cs_maj</t>
+          <t>C#</t>
         </is>
       </c>
     </row>
@@ -4309,7 +4309,7 @@
       </c>
       <c r="B395" t="inlineStr">
         <is>
-          <t>Cs_maj</t>
+          <t>C#</t>
         </is>
       </c>
     </row>
@@ -4319,7 +4319,7 @@
       </c>
       <c r="B396" t="inlineStr">
         <is>
-          <t>Cs_maj</t>
+          <t>C#</t>
         </is>
       </c>
     </row>
@@ -4329,7 +4329,7 @@
       </c>
       <c r="B397" t="inlineStr">
         <is>
-          <t>Cs_maj</t>
+          <t>C#</t>
         </is>
       </c>
     </row>
@@ -4339,7 +4339,7 @@
       </c>
       <c r="B398" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -4349,7 +4349,7 @@
       </c>
       <c r="B399" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -4359,7 +4359,7 @@
       </c>
       <c r="B400" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -4369,7 +4369,7 @@
       </c>
       <c r="B401" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -4379,7 +4379,7 @@
       </c>
       <c r="B402" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -4389,7 +4389,7 @@
       </c>
       <c r="B403" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -4399,7 +4399,7 @@
       </c>
       <c r="B404" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -4409,7 +4409,7 @@
       </c>
       <c r="B405" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -4419,7 +4419,7 @@
       </c>
       <c r="B406" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -4429,7 +4429,7 @@
       </c>
       <c r="B407" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -4439,7 +4439,7 @@
       </c>
       <c r="B408" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -4449,7 +4449,7 @@
       </c>
       <c r="B409" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -4459,7 +4459,7 @@
       </c>
       <c r="B410" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -4469,7 +4469,7 @@
       </c>
       <c r="B411" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -4479,7 +4479,7 @@
       </c>
       <c r="B412" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -4489,7 +4489,7 @@
       </c>
       <c r="B413" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -4499,7 +4499,7 @@
       </c>
       <c r="B414" t="inlineStr">
         <is>
-          <t>Fs_min</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed issue with __pycache__
</commit_message>
<xml_diff>
--- a/chords.xlsx
+++ b/chords.xlsx
@@ -14,24 +14,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="7">
   <si>
     <t>Chords</t>
+  </si>
+  <si>
+    <t>rest</t>
   </si>
   <si>
     <t>Bm</t>
   </si>
   <si>
+    <t>G</t>
+  </si>
+  <si>
     <t>F#</t>
   </si>
   <si>
-    <t>E</t>
+    <t>Em</t>
   </si>
   <si>
-    <t>F#7</t>
-  </si>
-  <si>
-    <t>rest</t>
+    <t>A</t>
   </si>
 </sst>
 </file>
@@ -389,7 +392,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B476"/>
+  <dimension ref="A1:B435"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -437,7 +440,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -445,7 +448,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -469,7 +472,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -477,7 +480,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -485,7 +488,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -493,7 +496,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -501,7 +504,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -509,7 +512,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -517,7 +520,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -525,7 +528,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -533,7 +536,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -541,7 +544,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -549,7 +552,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -557,7 +560,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -565,7 +568,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -573,7 +576,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -597,7 +600,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -605,7 +608,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -613,7 +616,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -621,7 +624,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -629,7 +632,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -637,7 +640,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -645,7 +648,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -653,7 +656,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -661,7 +664,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -669,7 +672,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -677,7 +680,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -685,7 +688,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -693,7 +696,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -701,7 +704,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -725,7 +728,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -733,7 +736,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -741,7 +744,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -749,7 +752,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -757,7 +760,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -765,7 +768,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -773,7 +776,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -781,7 +784,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -789,7 +792,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -797,7 +800,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -805,7 +808,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -813,7 +816,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -821,7 +824,7 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -829,7 +832,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -853,7 +856,7 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -861,7 +864,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -869,7 +872,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -877,7 +880,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -885,7 +888,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -893,7 +896,7 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -901,7 +904,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -909,7 +912,7 @@
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -917,7 +920,7 @@
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -925,7 +928,7 @@
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -933,7 +936,7 @@
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -941,7 +944,7 @@
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -949,7 +952,7 @@
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -957,7 +960,7 @@
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -981,7 +984,7 @@
         <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -989,7 +992,7 @@
         <v>73</v>
       </c>
       <c r="B75" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -997,7 +1000,7 @@
         <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -1005,7 +1008,7 @@
         <v>75</v>
       </c>
       <c r="B77" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -1013,7 +1016,7 @@
         <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -1021,7 +1024,7 @@
         <v>77</v>
       </c>
       <c r="B79" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -1029,7 +1032,7 @@
         <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -1037,7 +1040,7 @@
         <v>79</v>
       </c>
       <c r="B81" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -1045,7 +1048,7 @@
         <v>80</v>
       </c>
       <c r="B82" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1053,7 +1056,7 @@
         <v>81</v>
       </c>
       <c r="B83" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -1061,7 +1064,7 @@
         <v>82</v>
       </c>
       <c r="B84" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -1069,7 +1072,7 @@
         <v>83</v>
       </c>
       <c r="B85" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -1077,7 +1080,7 @@
         <v>84</v>
       </c>
       <c r="B86" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -1085,7 +1088,7 @@
         <v>85</v>
       </c>
       <c r="B87" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -1109,7 +1112,7 @@
         <v>88</v>
       </c>
       <c r="B90" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -1117,7 +1120,7 @@
         <v>89</v>
       </c>
       <c r="B91" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -1125,7 +1128,7 @@
         <v>90</v>
       </c>
       <c r="B92" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -1133,7 +1136,7 @@
         <v>91</v>
       </c>
       <c r="B93" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -1141,7 +1144,7 @@
         <v>92</v>
       </c>
       <c r="B94" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -1149,7 +1152,7 @@
         <v>93</v>
       </c>
       <c r="B95" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -1157,7 +1160,7 @@
         <v>94</v>
       </c>
       <c r="B96" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -1165,7 +1168,7 @@
         <v>95</v>
       </c>
       <c r="B97" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -1173,7 +1176,7 @@
         <v>96</v>
       </c>
       <c r="B98" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -1181,7 +1184,7 @@
         <v>97</v>
       </c>
       <c r="B99" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -1189,7 +1192,7 @@
         <v>98</v>
       </c>
       <c r="B100" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -1197,7 +1200,7 @@
         <v>99</v>
       </c>
       <c r="B101" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -1205,7 +1208,7 @@
         <v>100</v>
       </c>
       <c r="B102" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -1213,7 +1216,7 @@
         <v>101</v>
       </c>
       <c r="B103" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -1237,7 +1240,7 @@
         <v>104</v>
       </c>
       <c r="B106" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -1245,7 +1248,7 @@
         <v>105</v>
       </c>
       <c r="B107" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -1253,7 +1256,7 @@
         <v>106</v>
       </c>
       <c r="B108" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -1261,7 +1264,7 @@
         <v>107</v>
       </c>
       <c r="B109" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -1269,7 +1272,7 @@
         <v>108</v>
       </c>
       <c r="B110" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -1277,7 +1280,7 @@
         <v>109</v>
       </c>
       <c r="B111" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -1285,7 +1288,7 @@
         <v>110</v>
       </c>
       <c r="B112" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -1293,7 +1296,7 @@
         <v>111</v>
       </c>
       <c r="B113" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -1301,7 +1304,7 @@
         <v>112</v>
       </c>
       <c r="B114" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -1309,7 +1312,7 @@
         <v>113</v>
       </c>
       <c r="B115" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -1317,7 +1320,7 @@
         <v>114</v>
       </c>
       <c r="B116" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -1325,7 +1328,7 @@
         <v>115</v>
       </c>
       <c r="B117" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="118" spans="1:2">
@@ -1333,7 +1336,7 @@
         <v>116</v>
       </c>
       <c r="B118" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -1341,7 +1344,7 @@
         <v>117</v>
       </c>
       <c r="B119" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -1349,7 +1352,7 @@
         <v>118</v>
       </c>
       <c r="B120" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -1357,7 +1360,7 @@
         <v>119</v>
       </c>
       <c r="B121" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -1365,7 +1368,7 @@
         <v>120</v>
       </c>
       <c r="B122" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -1373,7 +1376,7 @@
         <v>121</v>
       </c>
       <c r="B123" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="124" spans="1:2">
@@ -1381,7 +1384,7 @@
         <v>122</v>
       </c>
       <c r="B124" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -1389,7 +1392,7 @@
         <v>123</v>
       </c>
       <c r="B125" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="126" spans="1:2">
@@ -1397,7 +1400,7 @@
         <v>124</v>
       </c>
       <c r="B126" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="127" spans="1:2">
@@ -1405,7 +1408,7 @@
         <v>125</v>
       </c>
       <c r="B127" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -1413,7 +1416,7 @@
         <v>126</v>
       </c>
       <c r="B128" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -1421,7 +1424,7 @@
         <v>127</v>
       </c>
       <c r="B129" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -1429,7 +1432,7 @@
         <v>128</v>
       </c>
       <c r="B130" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -1437,7 +1440,7 @@
         <v>129</v>
       </c>
       <c r="B131" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -1445,7 +1448,7 @@
         <v>130</v>
       </c>
       <c r="B132" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -1453,7 +1456,7 @@
         <v>131</v>
       </c>
       <c r="B133" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -1461,7 +1464,7 @@
         <v>132</v>
       </c>
       <c r="B134" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="135" spans="1:2">
@@ -1469,7 +1472,7 @@
         <v>133</v>
       </c>
       <c r="B135" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="136" spans="1:2">
@@ -1477,7 +1480,7 @@
         <v>134</v>
       </c>
       <c r="B136" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -1485,7 +1488,7 @@
         <v>135</v>
       </c>
       <c r="B137" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -1493,7 +1496,7 @@
         <v>136</v>
       </c>
       <c r="B138" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -1501,7 +1504,7 @@
         <v>137</v>
       </c>
       <c r="B139" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -1509,7 +1512,7 @@
         <v>138</v>
       </c>
       <c r="B140" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="141" spans="1:2">
@@ -1517,7 +1520,7 @@
         <v>139</v>
       </c>
       <c r="B141" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="142" spans="1:2">
@@ -1525,7 +1528,7 @@
         <v>140</v>
       </c>
       <c r="B142" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="143" spans="1:2">
@@ -1533,7 +1536,7 @@
         <v>141</v>
       </c>
       <c r="B143" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="144" spans="1:2">
@@ -1541,7 +1544,7 @@
         <v>142</v>
       </c>
       <c r="B144" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -1549,7 +1552,7 @@
         <v>143</v>
       </c>
       <c r="B145" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -1557,7 +1560,7 @@
         <v>144</v>
       </c>
       <c r="B146" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="147" spans="1:2">
@@ -1565,7 +1568,7 @@
         <v>145</v>
       </c>
       <c r="B147" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="148" spans="1:2">
@@ -1589,7 +1592,7 @@
         <v>148</v>
       </c>
       <c r="B150" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="151" spans="1:2">
@@ -1597,7 +1600,7 @@
         <v>149</v>
       </c>
       <c r="B151" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="152" spans="1:2">
@@ -1605,7 +1608,7 @@
         <v>150</v>
       </c>
       <c r="B152" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="153" spans="1:2">
@@ -1613,7 +1616,7 @@
         <v>151</v>
       </c>
       <c r="B153" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="154" spans="1:2">
@@ -1621,7 +1624,7 @@
         <v>152</v>
       </c>
       <c r="B154" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="155" spans="1:2">
@@ -1629,7 +1632,7 @@
         <v>153</v>
       </c>
       <c r="B155" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="156" spans="1:2">
@@ -1637,7 +1640,7 @@
         <v>154</v>
       </c>
       <c r="B156" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="157" spans="1:2">
@@ -1645,7 +1648,7 @@
         <v>155</v>
       </c>
       <c r="B157" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="158" spans="1:2">
@@ -1653,7 +1656,7 @@
         <v>156</v>
       </c>
       <c r="B158" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="159" spans="1:2">
@@ -1661,7 +1664,7 @@
         <v>157</v>
       </c>
       <c r="B159" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="160" spans="1:2">
@@ -1669,7 +1672,7 @@
         <v>158</v>
       </c>
       <c r="B160" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="161" spans="1:2">
@@ -1677,7 +1680,7 @@
         <v>159</v>
       </c>
       <c r="B161" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="162" spans="1:2">
@@ -1685,7 +1688,7 @@
         <v>160</v>
       </c>
       <c r="B162" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="163" spans="1:2">
@@ -1693,7 +1696,7 @@
         <v>161</v>
       </c>
       <c r="B163" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="164" spans="1:2">
@@ -1701,7 +1704,7 @@
         <v>162</v>
       </c>
       <c r="B164" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="165" spans="1:2">
@@ -1709,7 +1712,7 @@
         <v>163</v>
       </c>
       <c r="B165" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="166" spans="1:2">
@@ -1717,7 +1720,7 @@
         <v>164</v>
       </c>
       <c r="B166" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="167" spans="1:2">
@@ -1725,7 +1728,7 @@
         <v>165</v>
       </c>
       <c r="B167" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="168" spans="1:2">
@@ -1733,7 +1736,7 @@
         <v>166</v>
       </c>
       <c r="B168" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="169" spans="1:2">
@@ -1741,7 +1744,7 @@
         <v>167</v>
       </c>
       <c r="B169" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="170" spans="1:2">
@@ -1749,7 +1752,7 @@
         <v>168</v>
       </c>
       <c r="B170" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="171" spans="1:2">
@@ -1757,7 +1760,7 @@
         <v>169</v>
       </c>
       <c r="B171" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="172" spans="1:2">
@@ -1765,7 +1768,7 @@
         <v>170</v>
       </c>
       <c r="B172" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="173" spans="1:2">
@@ -1773,7 +1776,7 @@
         <v>171</v>
       </c>
       <c r="B173" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="174" spans="1:2">
@@ -1781,7 +1784,7 @@
         <v>172</v>
       </c>
       <c r="B174" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="175" spans="1:2">
@@ -1789,7 +1792,7 @@
         <v>173</v>
       </c>
       <c r="B175" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="176" spans="1:2">
@@ -1797,7 +1800,7 @@
         <v>174</v>
       </c>
       <c r="B176" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="177" spans="1:2">
@@ -1805,7 +1808,7 @@
         <v>175</v>
       </c>
       <c r="B177" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="178" spans="1:2">
@@ -1813,7 +1816,7 @@
         <v>176</v>
       </c>
       <c r="B178" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="179" spans="1:2">
@@ -1821,7 +1824,7 @@
         <v>177</v>
       </c>
       <c r="B179" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="180" spans="1:2">
@@ -1829,7 +1832,7 @@
         <v>178</v>
       </c>
       <c r="B180" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="181" spans="1:2">
@@ -1837,7 +1840,7 @@
         <v>179</v>
       </c>
       <c r="B181" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="182" spans="1:2">
@@ -1845,7 +1848,7 @@
         <v>180</v>
       </c>
       <c r="B182" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="183" spans="1:2">
@@ -1853,7 +1856,7 @@
         <v>181</v>
       </c>
       <c r="B183" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="184" spans="1:2">
@@ -1861,7 +1864,7 @@
         <v>182</v>
       </c>
       <c r="B184" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="185" spans="1:2">
@@ -1869,7 +1872,7 @@
         <v>183</v>
       </c>
       <c r="B185" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="186" spans="1:2">
@@ -1877,7 +1880,7 @@
         <v>184</v>
       </c>
       <c r="B186" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="187" spans="1:2">
@@ -1885,7 +1888,7 @@
         <v>185</v>
       </c>
       <c r="B187" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="188" spans="1:2">
@@ -1893,7 +1896,7 @@
         <v>186</v>
       </c>
       <c r="B188" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="189" spans="1:2">
@@ -1901,7 +1904,7 @@
         <v>187</v>
       </c>
       <c r="B189" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="190" spans="1:2">
@@ -1909,7 +1912,7 @@
         <v>188</v>
       </c>
       <c r="B190" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="191" spans="1:2">
@@ -1917,7 +1920,7 @@
         <v>189</v>
       </c>
       <c r="B191" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="192" spans="1:2">
@@ -1925,7 +1928,7 @@
         <v>190</v>
       </c>
       <c r="B192" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="193" spans="1:2">
@@ -1933,7 +1936,7 @@
         <v>191</v>
       </c>
       <c r="B193" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="194" spans="1:2">
@@ -1941,7 +1944,7 @@
         <v>192</v>
       </c>
       <c r="B194" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="195" spans="1:2">
@@ -1949,7 +1952,7 @@
         <v>193</v>
       </c>
       <c r="B195" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="196" spans="1:2">
@@ -1957,7 +1960,7 @@
         <v>194</v>
       </c>
       <c r="B196" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="197" spans="1:2">
@@ -1965,7 +1968,7 @@
         <v>195</v>
       </c>
       <c r="B197" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="198" spans="1:2">
@@ -1973,7 +1976,7 @@
         <v>196</v>
       </c>
       <c r="B198" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="199" spans="1:2">
@@ -1981,7 +1984,7 @@
         <v>197</v>
       </c>
       <c r="B199" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="200" spans="1:2">
@@ -1989,7 +1992,7 @@
         <v>198</v>
       </c>
       <c r="B200" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="201" spans="1:2">
@@ -1997,7 +2000,7 @@
         <v>199</v>
       </c>
       <c r="B201" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="202" spans="1:2">
@@ -2005,7 +2008,7 @@
         <v>200</v>
       </c>
       <c r="B202" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="203" spans="1:2">
@@ -2013,7 +2016,7 @@
         <v>201</v>
       </c>
       <c r="B203" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="204" spans="1:2">
@@ -2021,7 +2024,7 @@
         <v>202</v>
       </c>
       <c r="B204" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="205" spans="1:2">
@@ -2029,7 +2032,7 @@
         <v>203</v>
       </c>
       <c r="B205" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="206" spans="1:2">
@@ -2037,7 +2040,7 @@
         <v>204</v>
       </c>
       <c r="B206" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="207" spans="1:2">
@@ -2045,7 +2048,7 @@
         <v>205</v>
       </c>
       <c r="B207" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="208" spans="1:2">
@@ -2053,7 +2056,7 @@
         <v>206</v>
       </c>
       <c r="B208" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="209" spans="1:2">
@@ -2061,7 +2064,7 @@
         <v>207</v>
       </c>
       <c r="B209" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="210" spans="1:2">
@@ -2069,7 +2072,7 @@
         <v>208</v>
       </c>
       <c r="B210" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="211" spans="1:2">
@@ -2077,7 +2080,7 @@
         <v>209</v>
       </c>
       <c r="B211" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="212" spans="1:2">
@@ -2085,7 +2088,7 @@
         <v>210</v>
       </c>
       <c r="B212" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="213" spans="1:2">
@@ -2093,7 +2096,7 @@
         <v>211</v>
       </c>
       <c r="B213" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="214" spans="1:2">
@@ -2101,7 +2104,7 @@
         <v>212</v>
       </c>
       <c r="B214" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="215" spans="1:2">
@@ -2109,7 +2112,7 @@
         <v>213</v>
       </c>
       <c r="B215" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="216" spans="1:2">
@@ -2117,7 +2120,7 @@
         <v>214</v>
       </c>
       <c r="B216" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="217" spans="1:2">
@@ -2125,7 +2128,7 @@
         <v>215</v>
       </c>
       <c r="B217" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="218" spans="1:2">
@@ -2133,7 +2136,7 @@
         <v>216</v>
       </c>
       <c r="B218" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="219" spans="1:2">
@@ -2141,7 +2144,7 @@
         <v>217</v>
       </c>
       <c r="B219" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="220" spans="1:2">
@@ -2149,7 +2152,7 @@
         <v>218</v>
       </c>
       <c r="B220" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="221" spans="1:2">
@@ -2157,7 +2160,7 @@
         <v>219</v>
       </c>
       <c r="B221" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="222" spans="1:2">
@@ -2165,7 +2168,7 @@
         <v>220</v>
       </c>
       <c r="B222" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="223" spans="1:2">
@@ -2173,7 +2176,7 @@
         <v>221</v>
       </c>
       <c r="B223" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="224" spans="1:2">
@@ -2181,7 +2184,7 @@
         <v>222</v>
       </c>
       <c r="B224" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="225" spans="1:2">
@@ -2189,7 +2192,7 @@
         <v>223</v>
       </c>
       <c r="B225" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="226" spans="1:2">
@@ -2197,7 +2200,7 @@
         <v>224</v>
       </c>
       <c r="B226" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="227" spans="1:2">
@@ -2205,7 +2208,7 @@
         <v>225</v>
       </c>
       <c r="B227" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="228" spans="1:2">
@@ -2213,7 +2216,7 @@
         <v>226</v>
       </c>
       <c r="B228" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="229" spans="1:2">
@@ -2221,7 +2224,7 @@
         <v>227</v>
       </c>
       <c r="B229" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="230" spans="1:2">
@@ -2229,7 +2232,7 @@
         <v>228</v>
       </c>
       <c r="B230" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="231" spans="1:2">
@@ -2237,7 +2240,7 @@
         <v>229</v>
       </c>
       <c r="B231" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="232" spans="1:2">
@@ -2245,7 +2248,7 @@
         <v>230</v>
       </c>
       <c r="B232" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="233" spans="1:2">
@@ -2253,7 +2256,7 @@
         <v>231</v>
       </c>
       <c r="B233" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="234" spans="1:2">
@@ -2261,7 +2264,7 @@
         <v>232</v>
       </c>
       <c r="B234" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="235" spans="1:2">
@@ -2269,7 +2272,7 @@
         <v>233</v>
       </c>
       <c r="B235" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="236" spans="1:2">
@@ -2277,7 +2280,7 @@
         <v>234</v>
       </c>
       <c r="B236" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="237" spans="1:2">
@@ -2285,7 +2288,7 @@
         <v>235</v>
       </c>
       <c r="B237" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="238" spans="1:2">
@@ -2293,7 +2296,7 @@
         <v>236</v>
       </c>
       <c r="B238" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="239" spans="1:2">
@@ -2301,7 +2304,7 @@
         <v>237</v>
       </c>
       <c r="B239" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="240" spans="1:2">
@@ -2309,7 +2312,7 @@
         <v>238</v>
       </c>
       <c r="B240" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="241" spans="1:2">
@@ -2317,7 +2320,7 @@
         <v>239</v>
       </c>
       <c r="B241" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="242" spans="1:2">
@@ -2325,7 +2328,7 @@
         <v>240</v>
       </c>
       <c r="B242" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="243" spans="1:2">
@@ -2333,7 +2336,7 @@
         <v>241</v>
       </c>
       <c r="B243" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="244" spans="1:2">
@@ -2357,7 +2360,7 @@
         <v>244</v>
       </c>
       <c r="B246" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="247" spans="1:2">
@@ -2365,7 +2368,7 @@
         <v>245</v>
       </c>
       <c r="B247" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="248" spans="1:2">
@@ -2373,7 +2376,7 @@
         <v>246</v>
       </c>
       <c r="B248" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="249" spans="1:2">
@@ -2381,7 +2384,7 @@
         <v>247</v>
       </c>
       <c r="B249" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="250" spans="1:2">
@@ -2389,7 +2392,7 @@
         <v>248</v>
       </c>
       <c r="B250" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="251" spans="1:2">
@@ -2397,7 +2400,7 @@
         <v>249</v>
       </c>
       <c r="B251" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="252" spans="1:2">
@@ -2405,7 +2408,7 @@
         <v>250</v>
       </c>
       <c r="B252" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="253" spans="1:2">
@@ -2413,7 +2416,7 @@
         <v>251</v>
       </c>
       <c r="B253" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="254" spans="1:2">
@@ -2421,7 +2424,7 @@
         <v>252</v>
       </c>
       <c r="B254" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="255" spans="1:2">
@@ -2429,7 +2432,7 @@
         <v>253</v>
       </c>
       <c r="B255" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="256" spans="1:2">
@@ -2437,7 +2440,7 @@
         <v>254</v>
       </c>
       <c r="B256" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="257" spans="1:2">
@@ -2445,7 +2448,7 @@
         <v>255</v>
       </c>
       <c r="B257" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="258" spans="1:2">
@@ -2453,7 +2456,7 @@
         <v>256</v>
       </c>
       <c r="B258" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="259" spans="1:2">
@@ -2461,7 +2464,7 @@
         <v>257</v>
       </c>
       <c r="B259" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="260" spans="1:2">
@@ -2469,7 +2472,7 @@
         <v>258</v>
       </c>
       <c r="B260" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="261" spans="1:2">
@@ -2477,7 +2480,7 @@
         <v>259</v>
       </c>
       <c r="B261" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="262" spans="1:2">
@@ -2485,7 +2488,7 @@
         <v>260</v>
       </c>
       <c r="B262" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="263" spans="1:2">
@@ -2493,7 +2496,7 @@
         <v>261</v>
       </c>
       <c r="B263" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="264" spans="1:2">
@@ -2501,7 +2504,7 @@
         <v>262</v>
       </c>
       <c r="B264" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="265" spans="1:2">
@@ -2509,7 +2512,7 @@
         <v>263</v>
       </c>
       <c r="B265" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="266" spans="1:2">
@@ -2517,7 +2520,7 @@
         <v>264</v>
       </c>
       <c r="B266" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="267" spans="1:2">
@@ -2525,7 +2528,7 @@
         <v>265</v>
       </c>
       <c r="B267" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="268" spans="1:2">
@@ -2533,7 +2536,7 @@
         <v>266</v>
       </c>
       <c r="B268" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="269" spans="1:2">
@@ -2541,7 +2544,7 @@
         <v>267</v>
       </c>
       <c r="B269" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="270" spans="1:2">
@@ -2549,7 +2552,7 @@
         <v>268</v>
       </c>
       <c r="B270" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="271" spans="1:2">
@@ -2557,7 +2560,7 @@
         <v>269</v>
       </c>
       <c r="B271" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="272" spans="1:2">
@@ -2565,7 +2568,7 @@
         <v>270</v>
       </c>
       <c r="B272" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="273" spans="1:2">
@@ -2573,7 +2576,7 @@
         <v>271</v>
       </c>
       <c r="B273" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="274" spans="1:2">
@@ -2581,7 +2584,7 @@
         <v>272</v>
       </c>
       <c r="B274" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="275" spans="1:2">
@@ -2589,7 +2592,7 @@
         <v>273</v>
       </c>
       <c r="B275" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="276" spans="1:2">
@@ -2597,7 +2600,7 @@
         <v>274</v>
       </c>
       <c r="B276" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="277" spans="1:2">
@@ -2605,7 +2608,7 @@
         <v>275</v>
       </c>
       <c r="B277" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="278" spans="1:2">
@@ -2613,7 +2616,7 @@
         <v>276</v>
       </c>
       <c r="B278" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="279" spans="1:2">
@@ -2621,7 +2624,7 @@
         <v>277</v>
       </c>
       <c r="B279" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="280" spans="1:2">
@@ -2629,7 +2632,7 @@
         <v>278</v>
       </c>
       <c r="B280" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="281" spans="1:2">
@@ -2637,7 +2640,7 @@
         <v>279</v>
       </c>
       <c r="B281" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="282" spans="1:2">
@@ -2645,7 +2648,7 @@
         <v>280</v>
       </c>
       <c r="B282" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="283" spans="1:2">
@@ -2653,7 +2656,7 @@
         <v>281</v>
       </c>
       <c r="B283" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="284" spans="1:2">
@@ -2661,7 +2664,7 @@
         <v>282</v>
       </c>
       <c r="B284" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="285" spans="1:2">
@@ -2669,7 +2672,7 @@
         <v>283</v>
       </c>
       <c r="B285" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="286" spans="1:2">
@@ -2677,7 +2680,7 @@
         <v>284</v>
       </c>
       <c r="B286" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="287" spans="1:2">
@@ -2685,7 +2688,7 @@
         <v>285</v>
       </c>
       <c r="B287" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="288" spans="1:2">
@@ -2693,7 +2696,7 @@
         <v>286</v>
       </c>
       <c r="B288" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="289" spans="1:2">
@@ -2701,7 +2704,7 @@
         <v>287</v>
       </c>
       <c r="B289" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="290" spans="1:2">
@@ -2709,7 +2712,7 @@
         <v>288</v>
       </c>
       <c r="B290" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="291" spans="1:2">
@@ -2717,7 +2720,7 @@
         <v>289</v>
       </c>
       <c r="B291" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="292" spans="1:2">
@@ -2725,7 +2728,7 @@
         <v>290</v>
       </c>
       <c r="B292" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="293" spans="1:2">
@@ -2733,7 +2736,7 @@
         <v>291</v>
       </c>
       <c r="B293" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="294" spans="1:2">
@@ -2741,7 +2744,7 @@
         <v>292</v>
       </c>
       <c r="B294" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="295" spans="1:2">
@@ -2749,7 +2752,7 @@
         <v>293</v>
       </c>
       <c r="B295" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="296" spans="1:2">
@@ -2757,7 +2760,7 @@
         <v>294</v>
       </c>
       <c r="B296" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="297" spans="1:2">
@@ -2765,7 +2768,7 @@
         <v>295</v>
       </c>
       <c r="B297" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="298" spans="1:2">
@@ -2773,7 +2776,7 @@
         <v>296</v>
       </c>
       <c r="B298" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="299" spans="1:2">
@@ -2781,7 +2784,7 @@
         <v>297</v>
       </c>
       <c r="B299" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="300" spans="1:2">
@@ -2789,7 +2792,7 @@
         <v>298</v>
       </c>
       <c r="B300" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="301" spans="1:2">
@@ -2797,7 +2800,7 @@
         <v>299</v>
       </c>
       <c r="B301" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="302" spans="1:2">
@@ -2805,7 +2808,7 @@
         <v>300</v>
       </c>
       <c r="B302" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="303" spans="1:2">
@@ -2813,7 +2816,7 @@
         <v>301</v>
       </c>
       <c r="B303" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="304" spans="1:2">
@@ -2821,7 +2824,7 @@
         <v>302</v>
       </c>
       <c r="B304" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="305" spans="1:2">
@@ -2829,7 +2832,7 @@
         <v>303</v>
       </c>
       <c r="B305" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="306" spans="1:2">
@@ -2837,7 +2840,7 @@
         <v>304</v>
       </c>
       <c r="B306" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="307" spans="1:2">
@@ -2845,7 +2848,7 @@
         <v>305</v>
       </c>
       <c r="B307" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="308" spans="1:2">
@@ -2853,7 +2856,7 @@
         <v>306</v>
       </c>
       <c r="B308" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="309" spans="1:2">
@@ -2861,7 +2864,7 @@
         <v>307</v>
       </c>
       <c r="B309" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="310" spans="1:2">
@@ -2869,7 +2872,7 @@
         <v>308</v>
       </c>
       <c r="B310" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="311" spans="1:2">
@@ -2877,7 +2880,7 @@
         <v>309</v>
       </c>
       <c r="B311" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="312" spans="1:2">
@@ -2885,7 +2888,7 @@
         <v>310</v>
       </c>
       <c r="B312" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="313" spans="1:2">
@@ -2893,7 +2896,7 @@
         <v>311</v>
       </c>
       <c r="B313" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="314" spans="1:2">
@@ -2901,7 +2904,7 @@
         <v>312</v>
       </c>
       <c r="B314" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="315" spans="1:2">
@@ -2909,7 +2912,7 @@
         <v>313</v>
       </c>
       <c r="B315" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="316" spans="1:2">
@@ -2917,7 +2920,7 @@
         <v>314</v>
       </c>
       <c r="B316" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="317" spans="1:2">
@@ -2925,7 +2928,7 @@
         <v>315</v>
       </c>
       <c r="B317" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="318" spans="1:2">
@@ -2933,7 +2936,7 @@
         <v>316</v>
       </c>
       <c r="B318" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="319" spans="1:2">
@@ -2941,7 +2944,7 @@
         <v>317</v>
       </c>
       <c r="B319" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="320" spans="1:2">
@@ -2949,7 +2952,7 @@
         <v>318</v>
       </c>
       <c r="B320" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="321" spans="1:2">
@@ -2957,7 +2960,7 @@
         <v>319</v>
       </c>
       <c r="B321" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="322" spans="1:2">
@@ -2965,7 +2968,7 @@
         <v>320</v>
       </c>
       <c r="B322" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="323" spans="1:2">
@@ -2973,7 +2976,7 @@
         <v>321</v>
       </c>
       <c r="B323" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="324" spans="1:2">
@@ -2981,7 +2984,7 @@
         <v>322</v>
       </c>
       <c r="B324" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="325" spans="1:2">
@@ -2989,7 +2992,7 @@
         <v>323</v>
       </c>
       <c r="B325" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="326" spans="1:2">
@@ -2997,7 +3000,7 @@
         <v>324</v>
       </c>
       <c r="B326" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="327" spans="1:2">
@@ -3005,7 +3008,7 @@
         <v>325</v>
       </c>
       <c r="B327" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="328" spans="1:2">
@@ -3013,7 +3016,7 @@
         <v>326</v>
       </c>
       <c r="B328" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="329" spans="1:2">
@@ -3021,7 +3024,7 @@
         <v>327</v>
       </c>
       <c r="B329" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="330" spans="1:2">
@@ -3029,7 +3032,7 @@
         <v>328</v>
       </c>
       <c r="B330" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="331" spans="1:2">
@@ -3037,7 +3040,7 @@
         <v>329</v>
       </c>
       <c r="B331" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="332" spans="1:2">
@@ -3045,7 +3048,7 @@
         <v>330</v>
       </c>
       <c r="B332" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="333" spans="1:2">
@@ -3053,7 +3056,7 @@
         <v>331</v>
       </c>
       <c r="B333" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="334" spans="1:2">
@@ -3061,7 +3064,7 @@
         <v>332</v>
       </c>
       <c r="B334" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="335" spans="1:2">
@@ -3069,7 +3072,7 @@
         <v>333</v>
       </c>
       <c r="B335" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="336" spans="1:2">
@@ -3077,7 +3080,7 @@
         <v>334</v>
       </c>
       <c r="B336" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="337" spans="1:2">
@@ -3085,7 +3088,7 @@
         <v>335</v>
       </c>
       <c r="B337" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="338" spans="1:2">
@@ -3093,7 +3096,7 @@
         <v>336</v>
       </c>
       <c r="B338" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="339" spans="1:2">
@@ -3101,7 +3104,7 @@
         <v>337</v>
       </c>
       <c r="B339" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="340" spans="1:2">
@@ -3109,7 +3112,7 @@
         <v>338</v>
       </c>
       <c r="B340" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="341" spans="1:2">
@@ -3117,7 +3120,7 @@
         <v>339</v>
       </c>
       <c r="B341" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="342" spans="1:2">
@@ -3125,7 +3128,7 @@
         <v>340</v>
       </c>
       <c r="B342" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="343" spans="1:2">
@@ -3133,7 +3136,7 @@
         <v>341</v>
       </c>
       <c r="B343" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="344" spans="1:2">
@@ -3141,7 +3144,7 @@
         <v>342</v>
       </c>
       <c r="B344" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="345" spans="1:2">
@@ -3149,7 +3152,7 @@
         <v>343</v>
       </c>
       <c r="B345" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="346" spans="1:2">
@@ -3157,7 +3160,7 @@
         <v>344</v>
       </c>
       <c r="B346" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="347" spans="1:2">
@@ -3165,7 +3168,7 @@
         <v>345</v>
       </c>
       <c r="B347" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="348" spans="1:2">
@@ -3173,7 +3176,7 @@
         <v>346</v>
       </c>
       <c r="B348" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="349" spans="1:2">
@@ -3181,7 +3184,7 @@
         <v>347</v>
       </c>
       <c r="B349" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="350" spans="1:2">
@@ -3189,7 +3192,7 @@
         <v>348</v>
       </c>
       <c r="B350" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="351" spans="1:2">
@@ -3197,7 +3200,7 @@
         <v>349</v>
       </c>
       <c r="B351" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="352" spans="1:2">
@@ -3205,7 +3208,7 @@
         <v>350</v>
       </c>
       <c r="B352" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="353" spans="1:2">
@@ -3213,7 +3216,7 @@
         <v>351</v>
       </c>
       <c r="B353" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="354" spans="1:2">
@@ -3221,7 +3224,7 @@
         <v>352</v>
       </c>
       <c r="B354" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="355" spans="1:2">
@@ -3229,7 +3232,7 @@
         <v>353</v>
       </c>
       <c r="B355" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="356" spans="1:2">
@@ -3237,7 +3240,7 @@
         <v>354</v>
       </c>
       <c r="B356" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="357" spans="1:2">
@@ -3245,7 +3248,7 @@
         <v>355</v>
       </c>
       <c r="B357" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="358" spans="1:2">
@@ -3253,7 +3256,7 @@
         <v>356</v>
       </c>
       <c r="B358" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="359" spans="1:2">
@@ -3261,7 +3264,7 @@
         <v>357</v>
       </c>
       <c r="B359" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="360" spans="1:2">
@@ -3269,7 +3272,7 @@
         <v>358</v>
       </c>
       <c r="B360" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="361" spans="1:2">
@@ -3277,7 +3280,7 @@
         <v>359</v>
       </c>
       <c r="B361" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="362" spans="1:2">
@@ -3285,7 +3288,7 @@
         <v>360</v>
       </c>
       <c r="B362" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="363" spans="1:2">
@@ -3293,7 +3296,7 @@
         <v>361</v>
       </c>
       <c r="B363" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="364" spans="1:2">
@@ -3301,7 +3304,7 @@
         <v>362</v>
       </c>
       <c r="B364" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="365" spans="1:2">
@@ -3309,7 +3312,7 @@
         <v>363</v>
       </c>
       <c r="B365" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="366" spans="1:2">
@@ -3317,7 +3320,7 @@
         <v>364</v>
       </c>
       <c r="B366" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="367" spans="1:2">
@@ -3325,7 +3328,7 @@
         <v>365</v>
       </c>
       <c r="B367" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="368" spans="1:2">
@@ -3333,7 +3336,7 @@
         <v>366</v>
       </c>
       <c r="B368" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="369" spans="1:2">
@@ -3341,7 +3344,7 @@
         <v>367</v>
       </c>
       <c r="B369" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="370" spans="1:2">
@@ -3349,7 +3352,7 @@
         <v>368</v>
       </c>
       <c r="B370" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="371" spans="1:2">
@@ -3357,7 +3360,7 @@
         <v>369</v>
       </c>
       <c r="B371" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="372" spans="1:2">
@@ -3381,7 +3384,7 @@
         <v>372</v>
       </c>
       <c r="B374" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="375" spans="1:2">
@@ -3389,7 +3392,7 @@
         <v>373</v>
       </c>
       <c r="B375" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="376" spans="1:2">
@@ -3397,7 +3400,7 @@
         <v>374</v>
       </c>
       <c r="B376" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="377" spans="1:2">
@@ -3405,7 +3408,7 @@
         <v>375</v>
       </c>
       <c r="B377" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="378" spans="1:2">
@@ -3413,7 +3416,7 @@
         <v>376</v>
       </c>
       <c r="B378" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="379" spans="1:2">
@@ -3421,7 +3424,7 @@
         <v>377</v>
       </c>
       <c r="B379" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="380" spans="1:2">
@@ -3429,7 +3432,7 @@
         <v>378</v>
       </c>
       <c r="B380" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="381" spans="1:2">
@@ -3437,7 +3440,7 @@
         <v>379</v>
       </c>
       <c r="B381" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="382" spans="1:2">
@@ -3477,7 +3480,7 @@
         <v>384</v>
       </c>
       <c r="B386" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="387" spans="1:2">
@@ -3485,7 +3488,7 @@
         <v>385</v>
       </c>
       <c r="B387" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="388" spans="1:2">
@@ -3493,7 +3496,7 @@
         <v>386</v>
       </c>
       <c r="B388" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="389" spans="1:2">
@@ -3501,7 +3504,7 @@
         <v>387</v>
       </c>
       <c r="B389" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="390" spans="1:2">
@@ -3509,7 +3512,7 @@
         <v>388</v>
       </c>
       <c r="B390" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="391" spans="1:2">
@@ -3517,7 +3520,7 @@
         <v>389</v>
       </c>
       <c r="B391" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="392" spans="1:2">
@@ -3525,7 +3528,7 @@
         <v>390</v>
       </c>
       <c r="B392" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="393" spans="1:2">
@@ -3533,7 +3536,7 @@
         <v>391</v>
       </c>
       <c r="B393" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="394" spans="1:2">
@@ -3541,7 +3544,7 @@
         <v>392</v>
       </c>
       <c r="B394" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="395" spans="1:2">
@@ -3549,7 +3552,7 @@
         <v>393</v>
       </c>
       <c r="B395" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="396" spans="1:2">
@@ -3557,7 +3560,7 @@
         <v>394</v>
       </c>
       <c r="B396" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="397" spans="1:2">
@@ -3565,7 +3568,7 @@
         <v>395</v>
       </c>
       <c r="B397" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="398" spans="1:2">
@@ -3573,7 +3576,7 @@
         <v>396</v>
       </c>
       <c r="B398" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="399" spans="1:2">
@@ -3581,7 +3584,7 @@
         <v>397</v>
       </c>
       <c r="B399" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="400" spans="1:2">
@@ -3589,7 +3592,7 @@
         <v>398</v>
       </c>
       <c r="B400" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="401" spans="1:2">
@@ -3597,7 +3600,7 @@
         <v>399</v>
       </c>
       <c r="B401" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="402" spans="1:2">
@@ -3605,7 +3608,7 @@
         <v>400</v>
       </c>
       <c r="B402" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="403" spans="1:2">
@@ -3613,7 +3616,7 @@
         <v>401</v>
       </c>
       <c r="B403" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="404" spans="1:2">
@@ -3621,7 +3624,7 @@
         <v>402</v>
       </c>
       <c r="B404" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="405" spans="1:2">
@@ -3629,7 +3632,7 @@
         <v>403</v>
       </c>
       <c r="B405" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="406" spans="1:2">
@@ -3637,7 +3640,7 @@
         <v>404</v>
       </c>
       <c r="B406" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="407" spans="1:2">
@@ -3645,7 +3648,7 @@
         <v>405</v>
       </c>
       <c r="B407" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="408" spans="1:2">
@@ -3653,7 +3656,7 @@
         <v>406</v>
       </c>
       <c r="B408" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="409" spans="1:2">
@@ -3661,7 +3664,7 @@
         <v>407</v>
       </c>
       <c r="B409" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="410" spans="1:2">
@@ -3669,7 +3672,7 @@
         <v>408</v>
       </c>
       <c r="B410" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="411" spans="1:2">
@@ -3677,7 +3680,7 @@
         <v>409</v>
       </c>
       <c r="B411" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="412" spans="1:2">
@@ -3685,7 +3688,7 @@
         <v>410</v>
       </c>
       <c r="B412" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="413" spans="1:2">
@@ -3693,7 +3696,7 @@
         <v>411</v>
       </c>
       <c r="B413" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="414" spans="1:2">
@@ -3701,7 +3704,7 @@
         <v>412</v>
       </c>
       <c r="B414" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="415" spans="1:2">
@@ -3709,7 +3712,7 @@
         <v>413</v>
       </c>
       <c r="B415" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="416" spans="1:2">
@@ -3717,7 +3720,7 @@
         <v>414</v>
       </c>
       <c r="B416" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="417" spans="1:2">
@@ -3725,7 +3728,7 @@
         <v>415</v>
       </c>
       <c r="B417" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="418" spans="1:2">
@@ -3733,7 +3736,7 @@
         <v>416</v>
       </c>
       <c r="B418" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="419" spans="1:2">
@@ -3741,7 +3744,7 @@
         <v>417</v>
       </c>
       <c r="B419" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="420" spans="1:2">
@@ -3749,7 +3752,7 @@
         <v>418</v>
       </c>
       <c r="B420" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="421" spans="1:2">
@@ -3757,7 +3760,7 @@
         <v>419</v>
       </c>
       <c r="B421" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="422" spans="1:2">
@@ -3765,7 +3768,7 @@
         <v>420</v>
       </c>
       <c r="B422" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="423" spans="1:2">
@@ -3773,7 +3776,7 @@
         <v>421</v>
       </c>
       <c r="B423" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="424" spans="1:2">
@@ -3781,7 +3784,7 @@
         <v>422</v>
       </c>
       <c r="B424" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="425" spans="1:2">
@@ -3789,7 +3792,7 @@
         <v>423</v>
       </c>
       <c r="B425" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="426" spans="1:2">
@@ -3797,7 +3800,7 @@
         <v>424</v>
       </c>
       <c r="B426" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="427" spans="1:2">
@@ -3805,7 +3808,7 @@
         <v>425</v>
       </c>
       <c r="B427" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="428" spans="1:2">
@@ -3813,7 +3816,7 @@
         <v>426</v>
       </c>
       <c r="B428" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="429" spans="1:2">
@@ -3821,7 +3824,7 @@
         <v>427</v>
       </c>
       <c r="B429" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="430" spans="1:2">
@@ -3829,7 +3832,7 @@
         <v>428</v>
       </c>
       <c r="B430" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="431" spans="1:2">
@@ -3837,7 +3840,7 @@
         <v>429</v>
       </c>
       <c r="B431" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="432" spans="1:2">
@@ -3845,7 +3848,7 @@
         <v>430</v>
       </c>
       <c r="B432" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="433" spans="1:2">
@@ -3853,7 +3856,7 @@
         <v>431</v>
       </c>
       <c r="B433" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="434" spans="1:2">
@@ -3861,7 +3864,7 @@
         <v>432</v>
       </c>
       <c r="B434" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="435" spans="1:2">
@@ -3869,335 +3872,7 @@
         <v>433</v>
       </c>
       <c r="B435" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="436" spans="1:2">
-      <c r="A436" s="1">
-        <v>434</v>
-      </c>
-      <c r="B436" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="437" spans="1:2">
-      <c r="A437" s="1">
-        <v>435</v>
-      </c>
-      <c r="B437" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="438" spans="1:2">
-      <c r="A438" s="1">
-        <v>436</v>
-      </c>
-      <c r="B438" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="439" spans="1:2">
-      <c r="A439" s="1">
-        <v>437</v>
-      </c>
-      <c r="B439" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="440" spans="1:2">
-      <c r="A440" s="1">
-        <v>438</v>
-      </c>
-      <c r="B440" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="441" spans="1:2">
-      <c r="A441" s="1">
-        <v>439</v>
-      </c>
-      <c r="B441" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="442" spans="1:2">
-      <c r="A442" s="1">
-        <v>440</v>
-      </c>
-      <c r="B442" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="443" spans="1:2">
-      <c r="A443" s="1">
-        <v>441</v>
-      </c>
-      <c r="B443" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="444" spans="1:2">
-      <c r="A444" s="1">
-        <v>442</v>
-      </c>
-      <c r="B444" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="445" spans="1:2">
-      <c r="A445" s="1">
-        <v>443</v>
-      </c>
-      <c r="B445" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="446" spans="1:2">
-      <c r="A446" s="1">
-        <v>444</v>
-      </c>
-      <c r="B446" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="447" spans="1:2">
-      <c r="A447" s="1">
-        <v>445</v>
-      </c>
-      <c r="B447" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="448" spans="1:2">
-      <c r="A448" s="1">
-        <v>446</v>
-      </c>
-      <c r="B448" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="449" spans="1:2">
-      <c r="A449" s="1">
-        <v>447</v>
-      </c>
-      <c r="B449" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="450" spans="1:2">
-      <c r="A450" s="1">
-        <v>448</v>
-      </c>
-      <c r="B450" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="451" spans="1:2">
-      <c r="A451" s="1">
-        <v>449</v>
-      </c>
-      <c r="B451" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="452" spans="1:2">
-      <c r="A452" s="1">
-        <v>450</v>
-      </c>
-      <c r="B452" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="453" spans="1:2">
-      <c r="A453" s="1">
-        <v>451</v>
-      </c>
-      <c r="B453" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="454" spans="1:2">
-      <c r="A454" s="1">
-        <v>452</v>
-      </c>
-      <c r="B454" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="455" spans="1:2">
-      <c r="A455" s="1">
-        <v>453</v>
-      </c>
-      <c r="B455" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="456" spans="1:2">
-      <c r="A456" s="1">
-        <v>454</v>
-      </c>
-      <c r="B456" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="457" spans="1:2">
-      <c r="A457" s="1">
-        <v>455</v>
-      </c>
-      <c r="B457" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="458" spans="1:2">
-      <c r="A458" s="1">
-        <v>456</v>
-      </c>
-      <c r="B458" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="459" spans="1:2">
-      <c r="A459" s="1">
-        <v>457</v>
-      </c>
-      <c r="B459" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="460" spans="1:2">
-      <c r="A460" s="1">
-        <v>458</v>
-      </c>
-      <c r="B460" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="461" spans="1:2">
-      <c r="A461" s="1">
-        <v>459</v>
-      </c>
-      <c r="B461" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="462" spans="1:2">
-      <c r="A462" s="1">
-        <v>460</v>
-      </c>
-      <c r="B462" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="463" spans="1:2">
-      <c r="A463" s="1">
-        <v>461</v>
-      </c>
-      <c r="B463" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="464" spans="1:2">
-      <c r="A464" s="1">
-        <v>462</v>
-      </c>
-      <c r="B464" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="465" spans="1:2">
-      <c r="A465" s="1">
-        <v>463</v>
-      </c>
-      <c r="B465" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="466" spans="1:2">
-      <c r="A466" s="1">
-        <v>464</v>
-      </c>
-      <c r="B466" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="467" spans="1:2">
-      <c r="A467" s="1">
-        <v>465</v>
-      </c>
-      <c r="B467" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="468" spans="1:2">
-      <c r="A468" s="1">
-        <v>466</v>
-      </c>
-      <c r="B468" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="469" spans="1:2">
-      <c r="A469" s="1">
-        <v>467</v>
-      </c>
-      <c r="B469" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="470" spans="1:2">
-      <c r="A470" s="1">
-        <v>468</v>
-      </c>
-      <c r="B470" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="471" spans="1:2">
-      <c r="A471" s="1">
-        <v>469</v>
-      </c>
-      <c r="B471" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="472" spans="1:2">
-      <c r="A472" s="1">
-        <v>470</v>
-      </c>
-      <c r="B472" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="473" spans="1:2">
-      <c r="A473" s="1">
-        <v>471</v>
-      </c>
-      <c r="B473" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="474" spans="1:2">
-      <c r="A474" s="1">
-        <v>472</v>
-      </c>
-      <c r="B474" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="475" spans="1:2">
-      <c r="A475" s="1">
-        <v>473</v>
-      </c>
-      <c r="B475" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="476" spans="1:2">
-      <c r="A476" s="1">
-        <v>474</v>
-      </c>
-      <c r="B476" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Still working on getting code back up to its previous state
</commit_message>
<xml_diff>
--- a/chords.xlsx
+++ b/chords.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="12">
   <si>
     <t>Chords</t>
   </si>
@@ -22,16 +22,31 @@
     <t>rest</t>
   </si>
   <si>
-    <t>Bm</t>
+    <t>Gm</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Bb</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Dm</t>
+  </si>
+  <si>
+    <t>Em</t>
+  </si>
+  <si>
+    <t>Gb</t>
   </si>
   <si>
     <t>G</t>
   </si>
   <si>
-    <t>F#</t>
-  </si>
-  <si>
-    <t>Em</t>
+    <t>Am</t>
   </si>
   <si>
     <t>A</t>
@@ -392,7 +407,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B435"/>
+  <dimension ref="A1:B541"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -440,7 +455,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -448,7 +463,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -456,7 +471,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -464,7 +479,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -472,7 +487,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -480,7 +495,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -488,7 +503,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -496,7 +511,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -504,7 +519,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -512,7 +527,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -520,7 +535,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -528,7 +543,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -536,7 +551,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -544,7 +559,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -552,7 +567,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -560,7 +575,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -568,7 +583,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -576,7 +591,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -584,7 +599,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -592,7 +607,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -600,7 +615,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -608,7 +623,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -616,7 +631,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -624,7 +639,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -632,7 +647,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -640,7 +655,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -648,7 +663,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -656,7 +671,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -664,7 +679,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -672,7 +687,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -680,7 +695,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -688,7 +703,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -696,7 +711,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -704,7 +719,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -712,7 +727,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -720,7 +735,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -728,7 +743,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -736,7 +751,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -744,7 +759,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -752,7 +767,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -760,7 +775,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -768,7 +783,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -776,7 +791,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -784,7 +799,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -792,7 +807,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -800,7 +815,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -808,7 +823,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -816,7 +831,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -824,7 +839,7 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -832,7 +847,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -840,7 +855,7 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -848,7 +863,7 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -856,7 +871,7 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -864,7 +879,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -872,7 +887,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -880,7 +895,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -888,7 +903,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -896,7 +911,7 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -904,7 +919,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -912,7 +927,7 @@
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -920,7 +935,7 @@
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -928,7 +943,7 @@
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -936,7 +951,7 @@
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -944,7 +959,7 @@
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -952,7 +967,7 @@
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -960,7 +975,7 @@
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -968,7 +983,7 @@
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -976,7 +991,7 @@
         <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -984,7 +999,7 @@
         <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -992,7 +1007,7 @@
         <v>73</v>
       </c>
       <c r="B75" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -1000,7 +1015,7 @@
         <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -1008,7 +1023,7 @@
         <v>75</v>
       </c>
       <c r="B77" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -1016,7 +1031,7 @@
         <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -1024,7 +1039,7 @@
         <v>77</v>
       </c>
       <c r="B79" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -1032,7 +1047,7 @@
         <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -1040,7 +1055,7 @@
         <v>79</v>
       </c>
       <c r="B81" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -1048,7 +1063,7 @@
         <v>80</v>
       </c>
       <c r="B82" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1056,7 +1071,7 @@
         <v>81</v>
       </c>
       <c r="B83" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -1064,7 +1079,7 @@
         <v>82</v>
       </c>
       <c r="B84" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -1072,7 +1087,7 @@
         <v>83</v>
       </c>
       <c r="B85" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -1080,7 +1095,7 @@
         <v>84</v>
       </c>
       <c r="B86" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -1088,7 +1103,7 @@
         <v>85</v>
       </c>
       <c r="B87" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -1096,7 +1111,7 @@
         <v>86</v>
       </c>
       <c r="B88" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -1104,7 +1119,7 @@
         <v>87</v>
       </c>
       <c r="B89" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -1112,7 +1127,7 @@
         <v>88</v>
       </c>
       <c r="B90" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -1120,7 +1135,7 @@
         <v>89</v>
       </c>
       <c r="B91" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -1128,7 +1143,7 @@
         <v>90</v>
       </c>
       <c r="B92" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -1136,7 +1151,7 @@
         <v>91</v>
       </c>
       <c r="B93" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -1144,7 +1159,7 @@
         <v>92</v>
       </c>
       <c r="B94" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -1152,7 +1167,7 @@
         <v>93</v>
       </c>
       <c r="B95" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -1160,7 +1175,7 @@
         <v>94</v>
       </c>
       <c r="B96" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -1168,7 +1183,7 @@
         <v>95</v>
       </c>
       <c r="B97" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -1176,7 +1191,7 @@
         <v>96</v>
       </c>
       <c r="B98" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -1184,7 +1199,7 @@
         <v>97</v>
       </c>
       <c r="B99" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -1192,7 +1207,7 @@
         <v>98</v>
       </c>
       <c r="B100" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -1200,7 +1215,7 @@
         <v>99</v>
       </c>
       <c r="B101" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -1208,7 +1223,7 @@
         <v>100</v>
       </c>
       <c r="B102" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -1216,7 +1231,7 @@
         <v>101</v>
       </c>
       <c r="B103" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -1224,7 +1239,7 @@
         <v>102</v>
       </c>
       <c r="B104" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -1232,7 +1247,7 @@
         <v>103</v>
       </c>
       <c r="B105" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -1240,7 +1255,7 @@
         <v>104</v>
       </c>
       <c r="B106" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -1248,7 +1263,7 @@
         <v>105</v>
       </c>
       <c r="B107" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -1256,7 +1271,7 @@
         <v>106</v>
       </c>
       <c r="B108" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -1264,7 +1279,7 @@
         <v>107</v>
       </c>
       <c r="B109" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -1272,7 +1287,7 @@
         <v>108</v>
       </c>
       <c r="B110" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -1280,7 +1295,7 @@
         <v>109</v>
       </c>
       <c r="B111" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -1288,7 +1303,7 @@
         <v>110</v>
       </c>
       <c r="B112" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -1296,7 +1311,7 @@
         <v>111</v>
       </c>
       <c r="B113" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -1304,7 +1319,7 @@
         <v>112</v>
       </c>
       <c r="B114" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -1312,7 +1327,7 @@
         <v>113</v>
       </c>
       <c r="B115" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -1320,7 +1335,7 @@
         <v>114</v>
       </c>
       <c r="B116" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -1328,7 +1343,7 @@
         <v>115</v>
       </c>
       <c r="B117" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="118" spans="1:2">
@@ -1336,7 +1351,7 @@
         <v>116</v>
       </c>
       <c r="B118" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -1344,7 +1359,7 @@
         <v>117</v>
       </c>
       <c r="B119" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -1352,7 +1367,7 @@
         <v>118</v>
       </c>
       <c r="B120" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -1360,7 +1375,7 @@
         <v>119</v>
       </c>
       <c r="B121" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -1368,7 +1383,7 @@
         <v>120</v>
       </c>
       <c r="B122" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -1376,7 +1391,7 @@
         <v>121</v>
       </c>
       <c r="B123" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="124" spans="1:2">
@@ -1384,7 +1399,7 @@
         <v>122</v>
       </c>
       <c r="B124" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -1392,7 +1407,7 @@
         <v>123</v>
       </c>
       <c r="B125" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="126" spans="1:2">
@@ -1400,7 +1415,7 @@
         <v>124</v>
       </c>
       <c r="B126" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="127" spans="1:2">
@@ -1408,7 +1423,7 @@
         <v>125</v>
       </c>
       <c r="B127" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -1416,7 +1431,7 @@
         <v>126</v>
       </c>
       <c r="B128" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -1424,7 +1439,7 @@
         <v>127</v>
       </c>
       <c r="B129" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -1432,7 +1447,7 @@
         <v>128</v>
       </c>
       <c r="B130" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -1440,7 +1455,7 @@
         <v>129</v>
       </c>
       <c r="B131" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -1448,7 +1463,7 @@
         <v>130</v>
       </c>
       <c r="B132" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -1456,7 +1471,7 @@
         <v>131</v>
       </c>
       <c r="B133" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -1464,7 +1479,7 @@
         <v>132</v>
       </c>
       <c r="B134" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="135" spans="1:2">
@@ -1472,7 +1487,7 @@
         <v>133</v>
       </c>
       <c r="B135" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="136" spans="1:2">
@@ -1480,7 +1495,7 @@
         <v>134</v>
       </c>
       <c r="B136" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -1488,7 +1503,7 @@
         <v>135</v>
       </c>
       <c r="B137" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -1496,7 +1511,7 @@
         <v>136</v>
       </c>
       <c r="B138" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -1504,7 +1519,7 @@
         <v>137</v>
       </c>
       <c r="B139" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -1512,7 +1527,7 @@
         <v>138</v>
       </c>
       <c r="B140" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="141" spans="1:2">
@@ -1520,7 +1535,7 @@
         <v>139</v>
       </c>
       <c r="B141" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="142" spans="1:2">
@@ -1528,7 +1543,7 @@
         <v>140</v>
       </c>
       <c r="B142" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="143" spans="1:2">
@@ -1536,7 +1551,7 @@
         <v>141</v>
       </c>
       <c r="B143" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="144" spans="1:2">
@@ -1544,7 +1559,7 @@
         <v>142</v>
       </c>
       <c r="B144" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -1552,7 +1567,7 @@
         <v>143</v>
       </c>
       <c r="B145" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -1560,7 +1575,7 @@
         <v>144</v>
       </c>
       <c r="B146" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="147" spans="1:2">
@@ -1568,7 +1583,7 @@
         <v>145</v>
       </c>
       <c r="B147" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="148" spans="1:2">
@@ -1576,7 +1591,7 @@
         <v>146</v>
       </c>
       <c r="B148" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="149" spans="1:2">
@@ -1584,7 +1599,7 @@
         <v>147</v>
       </c>
       <c r="B149" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="150" spans="1:2">
@@ -1592,7 +1607,7 @@
         <v>148</v>
       </c>
       <c r="B150" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="151" spans="1:2">
@@ -1600,7 +1615,7 @@
         <v>149</v>
       </c>
       <c r="B151" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="152" spans="1:2">
@@ -1608,7 +1623,7 @@
         <v>150</v>
       </c>
       <c r="B152" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="153" spans="1:2">
@@ -1616,7 +1631,7 @@
         <v>151</v>
       </c>
       <c r="B153" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="154" spans="1:2">
@@ -1688,7 +1703,7 @@
         <v>160</v>
       </c>
       <c r="B162" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="163" spans="1:2">
@@ -1696,7 +1711,7 @@
         <v>161</v>
       </c>
       <c r="B163" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="164" spans="1:2">
@@ -1704,7 +1719,7 @@
         <v>162</v>
       </c>
       <c r="B164" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="165" spans="1:2">
@@ -1712,7 +1727,7 @@
         <v>163</v>
       </c>
       <c r="B165" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="166" spans="1:2">
@@ -1720,7 +1735,7 @@
         <v>164</v>
       </c>
       <c r="B166" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="167" spans="1:2">
@@ -1728,7 +1743,7 @@
         <v>165</v>
       </c>
       <c r="B167" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="168" spans="1:2">
@@ -1736,7 +1751,7 @@
         <v>166</v>
       </c>
       <c r="B168" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="169" spans="1:2">
@@ -1744,7 +1759,7 @@
         <v>167</v>
       </c>
       <c r="B169" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="170" spans="1:2">
@@ -1752,7 +1767,7 @@
         <v>168</v>
       </c>
       <c r="B170" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="171" spans="1:2">
@@ -1760,7 +1775,7 @@
         <v>169</v>
       </c>
       <c r="B171" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="172" spans="1:2">
@@ -1768,7 +1783,7 @@
         <v>170</v>
       </c>
       <c r="B172" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="173" spans="1:2">
@@ -1776,7 +1791,7 @@
         <v>171</v>
       </c>
       <c r="B173" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="174" spans="1:2">
@@ -1784,7 +1799,7 @@
         <v>172</v>
       </c>
       <c r="B174" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="175" spans="1:2">
@@ -1792,7 +1807,7 @@
         <v>173</v>
       </c>
       <c r="B175" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="176" spans="1:2">
@@ -1800,7 +1815,7 @@
         <v>174</v>
       </c>
       <c r="B176" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="177" spans="1:2">
@@ -1808,7 +1823,7 @@
         <v>175</v>
       </c>
       <c r="B177" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="178" spans="1:2">
@@ -1848,7 +1863,7 @@
         <v>180</v>
       </c>
       <c r="B182" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="183" spans="1:2">
@@ -1856,7 +1871,7 @@
         <v>181</v>
       </c>
       <c r="B183" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="184" spans="1:2">
@@ -1864,7 +1879,7 @@
         <v>182</v>
       </c>
       <c r="B184" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="185" spans="1:2">
@@ -1872,7 +1887,7 @@
         <v>183</v>
       </c>
       <c r="B185" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="186" spans="1:2">
@@ -1880,7 +1895,7 @@
         <v>184</v>
       </c>
       <c r="B186" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="187" spans="1:2">
@@ -1888,7 +1903,7 @@
         <v>185</v>
       </c>
       <c r="B187" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="188" spans="1:2">
@@ -1896,7 +1911,7 @@
         <v>186</v>
       </c>
       <c r="B188" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="189" spans="1:2">
@@ -1936,7 +1951,7 @@
         <v>191</v>
       </c>
       <c r="B193" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="194" spans="1:2">
@@ -1944,7 +1959,7 @@
         <v>192</v>
       </c>
       <c r="B194" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="195" spans="1:2">
@@ -1952,7 +1967,7 @@
         <v>193</v>
       </c>
       <c r="B195" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="196" spans="1:2">
@@ -1960,7 +1975,7 @@
         <v>194</v>
       </c>
       <c r="B196" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="197" spans="1:2">
@@ -1968,7 +1983,7 @@
         <v>195</v>
       </c>
       <c r="B197" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="198" spans="1:2">
@@ -1976,7 +1991,7 @@
         <v>196</v>
       </c>
       <c r="B198" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="199" spans="1:2">
@@ -1984,7 +1999,7 @@
         <v>197</v>
       </c>
       <c r="B199" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="200" spans="1:2">
@@ -1992,7 +2007,7 @@
         <v>198</v>
       </c>
       <c r="B200" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="201" spans="1:2">
@@ -2000,7 +2015,7 @@
         <v>199</v>
       </c>
       <c r="B201" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="202" spans="1:2">
@@ -2008,7 +2023,7 @@
         <v>200</v>
       </c>
       <c r="B202" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="203" spans="1:2">
@@ -2016,7 +2031,7 @@
         <v>201</v>
       </c>
       <c r="B203" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="204" spans="1:2">
@@ -2024,7 +2039,7 @@
         <v>202</v>
       </c>
       <c r="B204" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="205" spans="1:2">
@@ -2064,7 +2079,7 @@
         <v>207</v>
       </c>
       <c r="B209" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="210" spans="1:2">
@@ -2072,7 +2087,7 @@
         <v>208</v>
       </c>
       <c r="B210" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="211" spans="1:2">
@@ -2080,7 +2095,7 @@
         <v>209</v>
       </c>
       <c r="B211" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="212" spans="1:2">
@@ -2088,7 +2103,7 @@
         <v>210</v>
       </c>
       <c r="B212" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="213" spans="1:2">
@@ -2096,7 +2111,7 @@
         <v>211</v>
       </c>
       <c r="B213" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="214" spans="1:2">
@@ -2104,7 +2119,7 @@
         <v>212</v>
       </c>
       <c r="B214" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="215" spans="1:2">
@@ -2112,7 +2127,7 @@
         <v>213</v>
       </c>
       <c r="B215" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="216" spans="1:2">
@@ -2120,7 +2135,7 @@
         <v>214</v>
       </c>
       <c r="B216" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="217" spans="1:2">
@@ -2128,7 +2143,7 @@
         <v>215</v>
       </c>
       <c r="B217" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="218" spans="1:2">
@@ -2136,7 +2151,7 @@
         <v>216</v>
       </c>
       <c r="B218" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="219" spans="1:2">
@@ -2144,7 +2159,7 @@
         <v>217</v>
       </c>
       <c r="B219" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="220" spans="1:2">
@@ -2152,7 +2167,7 @@
         <v>218</v>
       </c>
       <c r="B220" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="221" spans="1:2">
@@ -2192,7 +2207,7 @@
         <v>223</v>
       </c>
       <c r="B225" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="226" spans="1:2">
@@ -2200,7 +2215,7 @@
         <v>224</v>
       </c>
       <c r="B226" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="227" spans="1:2">
@@ -2208,7 +2223,7 @@
         <v>225</v>
       </c>
       <c r="B227" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="228" spans="1:2">
@@ -2216,7 +2231,7 @@
         <v>226</v>
       </c>
       <c r="B228" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="229" spans="1:2">
@@ -2224,7 +2239,7 @@
         <v>227</v>
       </c>
       <c r="B229" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="230" spans="1:2">
@@ -2232,7 +2247,7 @@
         <v>228</v>
       </c>
       <c r="B230" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="231" spans="1:2">
@@ -2240,7 +2255,7 @@
         <v>229</v>
       </c>
       <c r="B231" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="232" spans="1:2">
@@ -2248,7 +2263,7 @@
         <v>230</v>
       </c>
       <c r="B232" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="233" spans="1:2">
@@ -2256,7 +2271,7 @@
         <v>231</v>
       </c>
       <c r="B233" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="234" spans="1:2">
@@ -2264,7 +2279,7 @@
         <v>232</v>
       </c>
       <c r="B234" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="235" spans="1:2">
@@ -2272,7 +2287,7 @@
         <v>233</v>
       </c>
       <c r="B235" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="236" spans="1:2">
@@ -2280,7 +2295,7 @@
         <v>234</v>
       </c>
       <c r="B236" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="237" spans="1:2">
@@ -2288,7 +2303,7 @@
         <v>235</v>
       </c>
       <c r="B237" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="238" spans="1:2">
@@ -2296,7 +2311,7 @@
         <v>236</v>
       </c>
       <c r="B238" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="239" spans="1:2">
@@ -2304,7 +2319,7 @@
         <v>237</v>
       </c>
       <c r="B239" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="240" spans="1:2">
@@ -2312,7 +2327,7 @@
         <v>238</v>
       </c>
       <c r="B240" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="241" spans="1:2">
@@ -2320,7 +2335,7 @@
         <v>239</v>
       </c>
       <c r="B241" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="242" spans="1:2">
@@ -2328,7 +2343,7 @@
         <v>240</v>
       </c>
       <c r="B242" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="243" spans="1:2">
@@ -2336,7 +2351,7 @@
         <v>241</v>
       </c>
       <c r="B243" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="244" spans="1:2">
@@ -2344,7 +2359,7 @@
         <v>242</v>
       </c>
       <c r="B244" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="245" spans="1:2">
@@ -2352,7 +2367,7 @@
         <v>243</v>
       </c>
       <c r="B245" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="246" spans="1:2">
@@ -2360,7 +2375,7 @@
         <v>244</v>
       </c>
       <c r="B246" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="247" spans="1:2">
@@ -2368,7 +2383,7 @@
         <v>245</v>
       </c>
       <c r="B247" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="248" spans="1:2">
@@ -2376,7 +2391,7 @@
         <v>246</v>
       </c>
       <c r="B248" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="249" spans="1:2">
@@ -2384,7 +2399,7 @@
         <v>247</v>
       </c>
       <c r="B249" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="250" spans="1:2">
@@ -2392,7 +2407,7 @@
         <v>248</v>
       </c>
       <c r="B250" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="251" spans="1:2">
@@ -2400,7 +2415,7 @@
         <v>249</v>
       </c>
       <c r="B251" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="252" spans="1:2">
@@ -2408,7 +2423,7 @@
         <v>250</v>
       </c>
       <c r="B252" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="253" spans="1:2">
@@ -2416,7 +2431,7 @@
         <v>251</v>
       </c>
       <c r="B253" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="254" spans="1:2">
@@ -2424,7 +2439,7 @@
         <v>252</v>
       </c>
       <c r="B254" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="255" spans="1:2">
@@ -2432,7 +2447,7 @@
         <v>253</v>
       </c>
       <c r="B255" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="256" spans="1:2">
@@ -2440,7 +2455,7 @@
         <v>254</v>
       </c>
       <c r="B256" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="257" spans="1:2">
@@ -2448,7 +2463,7 @@
         <v>255</v>
       </c>
       <c r="B257" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="258" spans="1:2">
@@ -2456,7 +2471,7 @@
         <v>256</v>
       </c>
       <c r="B258" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="259" spans="1:2">
@@ -2464,7 +2479,7 @@
         <v>257</v>
       </c>
       <c r="B259" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="260" spans="1:2">
@@ -2472,7 +2487,7 @@
         <v>258</v>
       </c>
       <c r="B260" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="261" spans="1:2">
@@ -2480,7 +2495,7 @@
         <v>259</v>
       </c>
       <c r="B261" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="262" spans="1:2">
@@ -2488,7 +2503,7 @@
         <v>260</v>
       </c>
       <c r="B262" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="263" spans="1:2">
@@ -2496,7 +2511,7 @@
         <v>261</v>
       </c>
       <c r="B263" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="264" spans="1:2">
@@ -2504,7 +2519,7 @@
         <v>262</v>
       </c>
       <c r="B264" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="265" spans="1:2">
@@ -2512,7 +2527,7 @@
         <v>263</v>
       </c>
       <c r="B265" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="266" spans="1:2">
@@ -2520,7 +2535,7 @@
         <v>264</v>
       </c>
       <c r="B266" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="267" spans="1:2">
@@ -2528,7 +2543,7 @@
         <v>265</v>
       </c>
       <c r="B267" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="268" spans="1:2">
@@ -2536,7 +2551,7 @@
         <v>266</v>
       </c>
       <c r="B268" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="269" spans="1:2">
@@ -2544,7 +2559,7 @@
         <v>267</v>
       </c>
       <c r="B269" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="270" spans="1:2">
@@ -2552,7 +2567,7 @@
         <v>268</v>
       </c>
       <c r="B270" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="271" spans="1:2">
@@ -2560,7 +2575,7 @@
         <v>269</v>
       </c>
       <c r="B271" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="272" spans="1:2">
@@ -2568,7 +2583,7 @@
         <v>270</v>
       </c>
       <c r="B272" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="273" spans="1:2">
@@ -2576,7 +2591,7 @@
         <v>271</v>
       </c>
       <c r="B273" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="274" spans="1:2">
@@ -2616,7 +2631,7 @@
         <v>276</v>
       </c>
       <c r="B278" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="279" spans="1:2">
@@ -2624,7 +2639,7 @@
         <v>277</v>
       </c>
       <c r="B279" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="280" spans="1:2">
@@ -2632,7 +2647,7 @@
         <v>278</v>
       </c>
       <c r="B280" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="281" spans="1:2">
@@ -2640,7 +2655,7 @@
         <v>279</v>
       </c>
       <c r="B281" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="282" spans="1:2">
@@ -2648,7 +2663,7 @@
         <v>280</v>
       </c>
       <c r="B282" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="283" spans="1:2">
@@ -2656,7 +2671,7 @@
         <v>281</v>
       </c>
       <c r="B283" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="284" spans="1:2">
@@ -2664,7 +2679,7 @@
         <v>282</v>
       </c>
       <c r="B284" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="285" spans="1:2">
@@ -2672,7 +2687,7 @@
         <v>283</v>
       </c>
       <c r="B285" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="286" spans="1:2">
@@ -2680,7 +2695,7 @@
         <v>284</v>
       </c>
       <c r="B286" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="287" spans="1:2">
@@ -2688,7 +2703,7 @@
         <v>285</v>
       </c>
       <c r="B287" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="288" spans="1:2">
@@ -2696,7 +2711,7 @@
         <v>286</v>
       </c>
       <c r="B288" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="289" spans="1:2">
@@ -2704,7 +2719,7 @@
         <v>287</v>
       </c>
       <c r="B289" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="290" spans="1:2">
@@ -2744,7 +2759,7 @@
         <v>292</v>
       </c>
       <c r="B294" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="295" spans="1:2">
@@ -2752,7 +2767,7 @@
         <v>293</v>
       </c>
       <c r="B295" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="296" spans="1:2">
@@ -2760,7 +2775,7 @@
         <v>294</v>
       </c>
       <c r="B296" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="297" spans="1:2">
@@ -2768,7 +2783,7 @@
         <v>295</v>
       </c>
       <c r="B297" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="298" spans="1:2">
@@ -2776,7 +2791,7 @@
         <v>296</v>
       </c>
       <c r="B298" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="299" spans="1:2">
@@ -2784,7 +2799,7 @@
         <v>297</v>
       </c>
       <c r="B299" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="300" spans="1:2">
@@ -2792,7 +2807,7 @@
         <v>298</v>
       </c>
       <c r="B300" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="301" spans="1:2">
@@ -2800,7 +2815,7 @@
         <v>299</v>
       </c>
       <c r="B301" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="302" spans="1:2">
@@ -2808,7 +2823,7 @@
         <v>300</v>
       </c>
       <c r="B302" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="303" spans="1:2">
@@ -2816,7 +2831,7 @@
         <v>301</v>
       </c>
       <c r="B303" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="304" spans="1:2">
@@ -2824,7 +2839,7 @@
         <v>302</v>
       </c>
       <c r="B304" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="305" spans="1:2">
@@ -2832,7 +2847,7 @@
         <v>303</v>
       </c>
       <c r="B305" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="306" spans="1:2">
@@ -2840,7 +2855,7 @@
         <v>304</v>
       </c>
       <c r="B306" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="307" spans="1:2">
@@ -2848,7 +2863,7 @@
         <v>305</v>
       </c>
       <c r="B307" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="308" spans="1:2">
@@ -2856,7 +2871,7 @@
         <v>306</v>
       </c>
       <c r="B308" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="309" spans="1:2">
@@ -2864,7 +2879,7 @@
         <v>307</v>
       </c>
       <c r="B309" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="310" spans="1:2">
@@ -2872,7 +2887,7 @@
         <v>308</v>
       </c>
       <c r="B310" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="311" spans="1:2">
@@ -2880,7 +2895,7 @@
         <v>309</v>
       </c>
       <c r="B311" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="312" spans="1:2">
@@ -2888,7 +2903,7 @@
         <v>310</v>
       </c>
       <c r="B312" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="313" spans="1:2">
@@ -2896,7 +2911,7 @@
         <v>311</v>
       </c>
       <c r="B313" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="314" spans="1:2">
@@ -2904,7 +2919,7 @@
         <v>312</v>
       </c>
       <c r="B314" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="315" spans="1:2">
@@ -2912,7 +2927,7 @@
         <v>313</v>
       </c>
       <c r="B315" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="316" spans="1:2">
@@ -2920,7 +2935,7 @@
         <v>314</v>
       </c>
       <c r="B316" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="317" spans="1:2">
@@ -2928,7 +2943,7 @@
         <v>315</v>
       </c>
       <c r="B317" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="318" spans="1:2">
@@ -2936,7 +2951,7 @@
         <v>316</v>
       </c>
       <c r="B318" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="319" spans="1:2">
@@ -2944,7 +2959,7 @@
         <v>317</v>
       </c>
       <c r="B319" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="320" spans="1:2">
@@ -2952,7 +2967,7 @@
         <v>318</v>
       </c>
       <c r="B320" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="321" spans="1:2">
@@ -2960,7 +2975,7 @@
         <v>319</v>
       </c>
       <c r="B321" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="322" spans="1:2">
@@ -2968,7 +2983,7 @@
         <v>320</v>
       </c>
       <c r="B322" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="323" spans="1:2">
@@ -2976,7 +2991,7 @@
         <v>321</v>
       </c>
       <c r="B323" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="324" spans="1:2">
@@ -2984,7 +2999,7 @@
         <v>322</v>
       </c>
       <c r="B324" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="325" spans="1:2">
@@ -2992,7 +3007,7 @@
         <v>323</v>
       </c>
       <c r="B325" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="326" spans="1:2">
@@ -3000,7 +3015,7 @@
         <v>324</v>
       </c>
       <c r="B326" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="327" spans="1:2">
@@ -3008,7 +3023,7 @@
         <v>325</v>
       </c>
       <c r="B327" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="328" spans="1:2">
@@ -3016,7 +3031,7 @@
         <v>326</v>
       </c>
       <c r="B328" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="329" spans="1:2">
@@ -3024,7 +3039,7 @@
         <v>327</v>
       </c>
       <c r="B329" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="330" spans="1:2">
@@ -3032,7 +3047,7 @@
         <v>328</v>
       </c>
       <c r="B330" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="331" spans="1:2">
@@ -3040,7 +3055,7 @@
         <v>329</v>
       </c>
       <c r="B331" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="332" spans="1:2">
@@ -3048,7 +3063,7 @@
         <v>330</v>
       </c>
       <c r="B332" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="333" spans="1:2">
@@ -3056,7 +3071,7 @@
         <v>331</v>
       </c>
       <c r="B333" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="334" spans="1:2">
@@ -3064,7 +3079,7 @@
         <v>332</v>
       </c>
       <c r="B334" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="335" spans="1:2">
@@ -3072,7 +3087,7 @@
         <v>333</v>
       </c>
       <c r="B335" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="336" spans="1:2">
@@ -3080,7 +3095,7 @@
         <v>334</v>
       </c>
       <c r="B336" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="337" spans="1:2">
@@ -3088,7 +3103,7 @@
         <v>335</v>
       </c>
       <c r="B337" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="338" spans="1:2">
@@ -3096,7 +3111,7 @@
         <v>336</v>
       </c>
       <c r="B338" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="339" spans="1:2">
@@ -3104,7 +3119,7 @@
         <v>337</v>
       </c>
       <c r="B339" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="340" spans="1:2">
@@ -3112,7 +3127,7 @@
         <v>338</v>
       </c>
       <c r="B340" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="341" spans="1:2">
@@ -3120,7 +3135,7 @@
         <v>339</v>
       </c>
       <c r="B341" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="342" spans="1:2">
@@ -3128,7 +3143,7 @@
         <v>340</v>
       </c>
       <c r="B342" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="343" spans="1:2">
@@ -3136,7 +3151,7 @@
         <v>341</v>
       </c>
       <c r="B343" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="344" spans="1:2">
@@ -3144,7 +3159,7 @@
         <v>342</v>
       </c>
       <c r="B344" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="345" spans="1:2">
@@ -3152,7 +3167,7 @@
         <v>343</v>
       </c>
       <c r="B345" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="346" spans="1:2">
@@ -3160,7 +3175,7 @@
         <v>344</v>
       </c>
       <c r="B346" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="347" spans="1:2">
@@ -3168,7 +3183,7 @@
         <v>345</v>
       </c>
       <c r="B347" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="348" spans="1:2">
@@ -3176,7 +3191,7 @@
         <v>346</v>
       </c>
       <c r="B348" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="349" spans="1:2">
@@ -3184,7 +3199,7 @@
         <v>347</v>
       </c>
       <c r="B349" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="350" spans="1:2">
@@ -3192,7 +3207,7 @@
         <v>348</v>
       </c>
       <c r="B350" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="351" spans="1:2">
@@ -3200,7 +3215,7 @@
         <v>349</v>
       </c>
       <c r="B351" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="352" spans="1:2">
@@ -3208,7 +3223,7 @@
         <v>350</v>
       </c>
       <c r="B352" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="353" spans="1:2">
@@ -3216,7 +3231,7 @@
         <v>351</v>
       </c>
       <c r="B353" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="354" spans="1:2">
@@ -3224,7 +3239,7 @@
         <v>352</v>
       </c>
       <c r="B354" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="355" spans="1:2">
@@ -3232,7 +3247,7 @@
         <v>353</v>
       </c>
       <c r="B355" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="356" spans="1:2">
@@ -3240,7 +3255,7 @@
         <v>354</v>
       </c>
       <c r="B356" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="357" spans="1:2">
@@ -3248,7 +3263,7 @@
         <v>355</v>
       </c>
       <c r="B357" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="358" spans="1:2">
@@ -3256,7 +3271,7 @@
         <v>356</v>
       </c>
       <c r="B358" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="359" spans="1:2">
@@ -3264,7 +3279,7 @@
         <v>357</v>
       </c>
       <c r="B359" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="360" spans="1:2">
@@ -3272,7 +3287,7 @@
         <v>358</v>
       </c>
       <c r="B360" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="361" spans="1:2">
@@ -3280,7 +3295,7 @@
         <v>359</v>
       </c>
       <c r="B361" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="362" spans="1:2">
@@ -3288,7 +3303,7 @@
         <v>360</v>
       </c>
       <c r="B362" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="363" spans="1:2">
@@ -3296,7 +3311,7 @@
         <v>361</v>
       </c>
       <c r="B363" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="364" spans="1:2">
@@ -3304,7 +3319,7 @@
         <v>362</v>
       </c>
       <c r="B364" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="365" spans="1:2">
@@ -3312,7 +3327,7 @@
         <v>363</v>
       </c>
       <c r="B365" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="366" spans="1:2">
@@ -3320,7 +3335,7 @@
         <v>364</v>
       </c>
       <c r="B366" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="367" spans="1:2">
@@ -3328,7 +3343,7 @@
         <v>365</v>
       </c>
       <c r="B367" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="368" spans="1:2">
@@ -3336,7 +3351,7 @@
         <v>366</v>
       </c>
       <c r="B368" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="369" spans="1:2">
@@ -3344,7 +3359,7 @@
         <v>367</v>
       </c>
       <c r="B369" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="370" spans="1:2">
@@ -3352,7 +3367,7 @@
         <v>368</v>
       </c>
       <c r="B370" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="371" spans="1:2">
@@ -3360,7 +3375,7 @@
         <v>369</v>
       </c>
       <c r="B371" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="372" spans="1:2">
@@ -3368,7 +3383,7 @@
         <v>370</v>
       </c>
       <c r="B372" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="373" spans="1:2">
@@ -3376,7 +3391,7 @@
         <v>371</v>
       </c>
       <c r="B373" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="374" spans="1:2">
@@ -3384,7 +3399,7 @@
         <v>372</v>
       </c>
       <c r="B374" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="375" spans="1:2">
@@ -3392,7 +3407,7 @@
         <v>373</v>
       </c>
       <c r="B375" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="376" spans="1:2">
@@ -3400,7 +3415,7 @@
         <v>374</v>
       </c>
       <c r="B376" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="377" spans="1:2">
@@ -3408,7 +3423,7 @@
         <v>375</v>
       </c>
       <c r="B377" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="378" spans="1:2">
@@ -3416,7 +3431,7 @@
         <v>376</v>
       </c>
       <c r="B378" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="379" spans="1:2">
@@ -3424,7 +3439,7 @@
         <v>377</v>
       </c>
       <c r="B379" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="380" spans="1:2">
@@ -3432,7 +3447,7 @@
         <v>378</v>
       </c>
       <c r="B380" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="381" spans="1:2">
@@ -3440,7 +3455,7 @@
         <v>379</v>
       </c>
       <c r="B381" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="382" spans="1:2">
@@ -3448,7 +3463,7 @@
         <v>380</v>
       </c>
       <c r="B382" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="383" spans="1:2">
@@ -3456,7 +3471,7 @@
         <v>381</v>
       </c>
       <c r="B383" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="384" spans="1:2">
@@ -3464,7 +3479,7 @@
         <v>382</v>
       </c>
       <c r="B384" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="385" spans="1:2">
@@ -3472,7 +3487,7 @@
         <v>383</v>
       </c>
       <c r="B385" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="386" spans="1:2">
@@ -3480,7 +3495,7 @@
         <v>384</v>
       </c>
       <c r="B386" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="387" spans="1:2">
@@ -3488,7 +3503,7 @@
         <v>385</v>
       </c>
       <c r="B387" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="388" spans="1:2">
@@ -3496,7 +3511,7 @@
         <v>386</v>
       </c>
       <c r="B388" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="389" spans="1:2">
@@ -3504,7 +3519,7 @@
         <v>387</v>
       </c>
       <c r="B389" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="390" spans="1:2">
@@ -3512,7 +3527,7 @@
         <v>388</v>
       </c>
       <c r="B390" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="391" spans="1:2">
@@ -3520,7 +3535,7 @@
         <v>389</v>
       </c>
       <c r="B391" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="392" spans="1:2">
@@ -3528,7 +3543,7 @@
         <v>390</v>
       </c>
       <c r="B392" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="393" spans="1:2">
@@ -3536,7 +3551,7 @@
         <v>391</v>
       </c>
       <c r="B393" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="394" spans="1:2">
@@ -3544,7 +3559,7 @@
         <v>392</v>
       </c>
       <c r="B394" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="395" spans="1:2">
@@ -3552,7 +3567,7 @@
         <v>393</v>
       </c>
       <c r="B395" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="396" spans="1:2">
@@ -3560,7 +3575,7 @@
         <v>394</v>
       </c>
       <c r="B396" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="397" spans="1:2">
@@ -3568,7 +3583,7 @@
         <v>395</v>
       </c>
       <c r="B397" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="398" spans="1:2">
@@ -3576,7 +3591,7 @@
         <v>396</v>
       </c>
       <c r="B398" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="399" spans="1:2">
@@ -3584,7 +3599,7 @@
         <v>397</v>
       </c>
       <c r="B399" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="400" spans="1:2">
@@ -3592,7 +3607,7 @@
         <v>398</v>
       </c>
       <c r="B400" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="401" spans="1:2">
@@ -3600,7 +3615,7 @@
         <v>399</v>
       </c>
       <c r="B401" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="402" spans="1:2">
@@ -3608,7 +3623,7 @@
         <v>400</v>
       </c>
       <c r="B402" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="403" spans="1:2">
@@ -3616,7 +3631,7 @@
         <v>401</v>
       </c>
       <c r="B403" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="404" spans="1:2">
@@ -3624,7 +3639,7 @@
         <v>402</v>
       </c>
       <c r="B404" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="405" spans="1:2">
@@ -3632,7 +3647,7 @@
         <v>403</v>
       </c>
       <c r="B405" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="406" spans="1:2">
@@ -3672,7 +3687,7 @@
         <v>408</v>
       </c>
       <c r="B410" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="411" spans="1:2">
@@ -3680,7 +3695,7 @@
         <v>409</v>
       </c>
       <c r="B411" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="412" spans="1:2">
@@ -3688,7 +3703,7 @@
         <v>410</v>
       </c>
       <c r="B412" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="413" spans="1:2">
@@ -3696,7 +3711,7 @@
         <v>411</v>
       </c>
       <c r="B413" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="414" spans="1:2">
@@ -3704,7 +3719,7 @@
         <v>412</v>
       </c>
       <c r="B414" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="415" spans="1:2">
@@ -3712,7 +3727,7 @@
         <v>413</v>
       </c>
       <c r="B415" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="416" spans="1:2">
@@ -3720,7 +3735,7 @@
         <v>414</v>
       </c>
       <c r="B416" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="417" spans="1:2">
@@ -3728,7 +3743,7 @@
         <v>415</v>
       </c>
       <c r="B417" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="418" spans="1:2">
@@ -3800,7 +3815,7 @@
         <v>424</v>
       </c>
       <c r="B426" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="427" spans="1:2">
@@ -3808,7 +3823,7 @@
         <v>425</v>
       </c>
       <c r="B427" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="428" spans="1:2">
@@ -3816,7 +3831,7 @@
         <v>426</v>
       </c>
       <c r="B428" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="429" spans="1:2">
@@ -3824,7 +3839,7 @@
         <v>427</v>
       </c>
       <c r="B429" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="430" spans="1:2">
@@ -3832,7 +3847,7 @@
         <v>428</v>
       </c>
       <c r="B430" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="431" spans="1:2">
@@ -3840,7 +3855,7 @@
         <v>429</v>
       </c>
       <c r="B431" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="432" spans="1:2">
@@ -3848,7 +3863,7 @@
         <v>430</v>
       </c>
       <c r="B432" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="433" spans="1:2">
@@ -3856,7 +3871,7 @@
         <v>431</v>
       </c>
       <c r="B433" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="434" spans="1:2">
@@ -3864,7 +3879,7 @@
         <v>432</v>
       </c>
       <c r="B434" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="435" spans="1:2">
@@ -3872,7 +3887,855 @@
         <v>433</v>
       </c>
       <c r="B435" t="s">
-        <v>1</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="436" spans="1:2">
+      <c r="A436" s="1">
+        <v>434</v>
+      </c>
+      <c r="B436" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="437" spans="1:2">
+      <c r="A437" s="1">
+        <v>435</v>
+      </c>
+      <c r="B437" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="438" spans="1:2">
+      <c r="A438" s="1">
+        <v>436</v>
+      </c>
+      <c r="B438" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="439" spans="1:2">
+      <c r="A439" s="1">
+        <v>437</v>
+      </c>
+      <c r="B439" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="440" spans="1:2">
+      <c r="A440" s="1">
+        <v>438</v>
+      </c>
+      <c r="B440" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="441" spans="1:2">
+      <c r="A441" s="1">
+        <v>439</v>
+      </c>
+      <c r="B441" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="442" spans="1:2">
+      <c r="A442" s="1">
+        <v>440</v>
+      </c>
+      <c r="B442" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="443" spans="1:2">
+      <c r="A443" s="1">
+        <v>441</v>
+      </c>
+      <c r="B443" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="444" spans="1:2">
+      <c r="A444" s="1">
+        <v>442</v>
+      </c>
+      <c r="B444" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="445" spans="1:2">
+      <c r="A445" s="1">
+        <v>443</v>
+      </c>
+      <c r="B445" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="446" spans="1:2">
+      <c r="A446" s="1">
+        <v>444</v>
+      </c>
+      <c r="B446" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="447" spans="1:2">
+      <c r="A447" s="1">
+        <v>445</v>
+      </c>
+      <c r="B447" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="448" spans="1:2">
+      <c r="A448" s="1">
+        <v>446</v>
+      </c>
+      <c r="B448" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="449" spans="1:2">
+      <c r="A449" s="1">
+        <v>447</v>
+      </c>
+      <c r="B449" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="450" spans="1:2">
+      <c r="A450" s="1">
+        <v>448</v>
+      </c>
+      <c r="B450" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="451" spans="1:2">
+      <c r="A451" s="1">
+        <v>449</v>
+      </c>
+      <c r="B451" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="452" spans="1:2">
+      <c r="A452" s="1">
+        <v>450</v>
+      </c>
+      <c r="B452" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="453" spans="1:2">
+      <c r="A453" s="1">
+        <v>451</v>
+      </c>
+      <c r="B453" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="454" spans="1:2">
+      <c r="A454" s="1">
+        <v>452</v>
+      </c>
+      <c r="B454" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="455" spans="1:2">
+      <c r="A455" s="1">
+        <v>453</v>
+      </c>
+      <c r="B455" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="456" spans="1:2">
+      <c r="A456" s="1">
+        <v>454</v>
+      </c>
+      <c r="B456" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="457" spans="1:2">
+      <c r="A457" s="1">
+        <v>455</v>
+      </c>
+      <c r="B457" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="458" spans="1:2">
+      <c r="A458" s="1">
+        <v>456</v>
+      </c>
+      <c r="B458" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="459" spans="1:2">
+      <c r="A459" s="1">
+        <v>457</v>
+      </c>
+      <c r="B459" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="460" spans="1:2">
+      <c r="A460" s="1">
+        <v>458</v>
+      </c>
+      <c r="B460" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="461" spans="1:2">
+      <c r="A461" s="1">
+        <v>459</v>
+      </c>
+      <c r="B461" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="462" spans="1:2">
+      <c r="A462" s="1">
+        <v>460</v>
+      </c>
+      <c r="B462" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="463" spans="1:2">
+      <c r="A463" s="1">
+        <v>461</v>
+      </c>
+      <c r="B463" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="464" spans="1:2">
+      <c r="A464" s="1">
+        <v>462</v>
+      </c>
+      <c r="B464" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="465" spans="1:2">
+      <c r="A465" s="1">
+        <v>463</v>
+      </c>
+      <c r="B465" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="466" spans="1:2">
+      <c r="A466" s="1">
+        <v>464</v>
+      </c>
+      <c r="B466" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="467" spans="1:2">
+      <c r="A467" s="1">
+        <v>465</v>
+      </c>
+      <c r="B467" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="468" spans="1:2">
+      <c r="A468" s="1">
+        <v>466</v>
+      </c>
+      <c r="B468" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="469" spans="1:2">
+      <c r="A469" s="1">
+        <v>467</v>
+      </c>
+      <c r="B469" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="470" spans="1:2">
+      <c r="A470" s="1">
+        <v>468</v>
+      </c>
+      <c r="B470" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="471" spans="1:2">
+      <c r="A471" s="1">
+        <v>469</v>
+      </c>
+      <c r="B471" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="472" spans="1:2">
+      <c r="A472" s="1">
+        <v>470</v>
+      </c>
+      <c r="B472" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="473" spans="1:2">
+      <c r="A473" s="1">
+        <v>471</v>
+      </c>
+      <c r="B473" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="474" spans="1:2">
+      <c r="A474" s="1">
+        <v>472</v>
+      </c>
+      <c r="B474" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="475" spans="1:2">
+      <c r="A475" s="1">
+        <v>473</v>
+      </c>
+      <c r="B475" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="476" spans="1:2">
+      <c r="A476" s="1">
+        <v>474</v>
+      </c>
+      <c r="B476" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="477" spans="1:2">
+      <c r="A477" s="1">
+        <v>475</v>
+      </c>
+      <c r="B477" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="478" spans="1:2">
+      <c r="A478" s="1">
+        <v>476</v>
+      </c>
+      <c r="B478" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="479" spans="1:2">
+      <c r="A479" s="1">
+        <v>477</v>
+      </c>
+      <c r="B479" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="480" spans="1:2">
+      <c r="A480" s="1">
+        <v>478</v>
+      </c>
+      <c r="B480" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="481" spans="1:2">
+      <c r="A481" s="1">
+        <v>479</v>
+      </c>
+      <c r="B481" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="482" spans="1:2">
+      <c r="A482" s="1">
+        <v>480</v>
+      </c>
+      <c r="B482" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="483" spans="1:2">
+      <c r="A483" s="1">
+        <v>481</v>
+      </c>
+      <c r="B483" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="484" spans="1:2">
+      <c r="A484" s="1">
+        <v>482</v>
+      </c>
+      <c r="B484" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="485" spans="1:2">
+      <c r="A485" s="1">
+        <v>483</v>
+      </c>
+      <c r="B485" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="486" spans="1:2">
+      <c r="A486" s="1">
+        <v>484</v>
+      </c>
+      <c r="B486" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="487" spans="1:2">
+      <c r="A487" s="1">
+        <v>485</v>
+      </c>
+      <c r="B487" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="488" spans="1:2">
+      <c r="A488" s="1">
+        <v>486</v>
+      </c>
+      <c r="B488" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="489" spans="1:2">
+      <c r="A489" s="1">
+        <v>487</v>
+      </c>
+      <c r="B489" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="490" spans="1:2">
+      <c r="A490" s="1">
+        <v>488</v>
+      </c>
+      <c r="B490" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="491" spans="1:2">
+      <c r="A491" s="1">
+        <v>489</v>
+      </c>
+      <c r="B491" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="492" spans="1:2">
+      <c r="A492" s="1">
+        <v>490</v>
+      </c>
+      <c r="B492" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="493" spans="1:2">
+      <c r="A493" s="1">
+        <v>491</v>
+      </c>
+      <c r="B493" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="494" spans="1:2">
+      <c r="A494" s="1">
+        <v>492</v>
+      </c>
+      <c r="B494" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="495" spans="1:2">
+      <c r="A495" s="1">
+        <v>493</v>
+      </c>
+      <c r="B495" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="496" spans="1:2">
+      <c r="A496" s="1">
+        <v>494</v>
+      </c>
+      <c r="B496" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="497" spans="1:2">
+      <c r="A497" s="1">
+        <v>495</v>
+      </c>
+      <c r="B497" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="498" spans="1:2">
+      <c r="A498" s="1">
+        <v>496</v>
+      </c>
+      <c r="B498" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="499" spans="1:2">
+      <c r="A499" s="1">
+        <v>497</v>
+      </c>
+      <c r="B499" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="500" spans="1:2">
+      <c r="A500" s="1">
+        <v>498</v>
+      </c>
+      <c r="B500" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="501" spans="1:2">
+      <c r="A501" s="1">
+        <v>499</v>
+      </c>
+      <c r="B501" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="502" spans="1:2">
+      <c r="A502" s="1">
+        <v>500</v>
+      </c>
+      <c r="B502" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="503" spans="1:2">
+      <c r="A503" s="1">
+        <v>501</v>
+      </c>
+      <c r="B503" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="504" spans="1:2">
+      <c r="A504" s="1">
+        <v>502</v>
+      </c>
+      <c r="B504" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="505" spans="1:2">
+      <c r="A505" s="1">
+        <v>503</v>
+      </c>
+      <c r="B505" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="506" spans="1:2">
+      <c r="A506" s="1">
+        <v>504</v>
+      </c>
+      <c r="B506" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="507" spans="1:2">
+      <c r="A507" s="1">
+        <v>505</v>
+      </c>
+      <c r="B507" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="508" spans="1:2">
+      <c r="A508" s="1">
+        <v>506</v>
+      </c>
+      <c r="B508" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="509" spans="1:2">
+      <c r="A509" s="1">
+        <v>507</v>
+      </c>
+      <c r="B509" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="510" spans="1:2">
+      <c r="A510" s="1">
+        <v>508</v>
+      </c>
+      <c r="B510" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="511" spans="1:2">
+      <c r="A511" s="1">
+        <v>509</v>
+      </c>
+      <c r="B511" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="512" spans="1:2">
+      <c r="A512" s="1">
+        <v>510</v>
+      </c>
+      <c r="B512" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="513" spans="1:2">
+      <c r="A513" s="1">
+        <v>511</v>
+      </c>
+      <c r="B513" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="514" spans="1:2">
+      <c r="A514" s="1">
+        <v>512</v>
+      </c>
+      <c r="B514" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="515" spans="1:2">
+      <c r="A515" s="1">
+        <v>513</v>
+      </c>
+      <c r="B515" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="516" spans="1:2">
+      <c r="A516" s="1">
+        <v>514</v>
+      </c>
+      <c r="B516" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="517" spans="1:2">
+      <c r="A517" s="1">
+        <v>515</v>
+      </c>
+      <c r="B517" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="518" spans="1:2">
+      <c r="A518" s="1">
+        <v>516</v>
+      </c>
+      <c r="B518" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="519" spans="1:2">
+      <c r="A519" s="1">
+        <v>517</v>
+      </c>
+      <c r="B519" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="520" spans="1:2">
+      <c r="A520" s="1">
+        <v>518</v>
+      </c>
+      <c r="B520" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="521" spans="1:2">
+      <c r="A521" s="1">
+        <v>519</v>
+      </c>
+      <c r="B521" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="522" spans="1:2">
+      <c r="A522" s="1">
+        <v>520</v>
+      </c>
+      <c r="B522" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="523" spans="1:2">
+      <c r="A523" s="1">
+        <v>521</v>
+      </c>
+      <c r="B523" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="524" spans="1:2">
+      <c r="A524" s="1">
+        <v>522</v>
+      </c>
+      <c r="B524" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="525" spans="1:2">
+      <c r="A525" s="1">
+        <v>523</v>
+      </c>
+      <c r="B525" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="526" spans="1:2">
+      <c r="A526" s="1">
+        <v>524</v>
+      </c>
+      <c r="B526" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="527" spans="1:2">
+      <c r="A527" s="1">
+        <v>525</v>
+      </c>
+      <c r="B527" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="528" spans="1:2">
+      <c r="A528" s="1">
+        <v>526</v>
+      </c>
+      <c r="B528" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="529" spans="1:2">
+      <c r="A529" s="1">
+        <v>527</v>
+      </c>
+      <c r="B529" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="530" spans="1:2">
+      <c r="A530" s="1">
+        <v>528</v>
+      </c>
+      <c r="B530" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="531" spans="1:2">
+      <c r="A531" s="1">
+        <v>529</v>
+      </c>
+      <c r="B531" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="532" spans="1:2">
+      <c r="A532" s="1">
+        <v>530</v>
+      </c>
+      <c r="B532" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="533" spans="1:2">
+      <c r="A533" s="1">
+        <v>531</v>
+      </c>
+      <c r="B533" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="534" spans="1:2">
+      <c r="A534" s="1">
+        <v>532</v>
+      </c>
+      <c r="B534" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="535" spans="1:2">
+      <c r="A535" s="1">
+        <v>533</v>
+      </c>
+      <c r="B535" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="536" spans="1:2">
+      <c r="A536" s="1">
+        <v>534</v>
+      </c>
+      <c r="B536" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="537" spans="1:2">
+      <c r="A537" s="1">
+        <v>535</v>
+      </c>
+      <c r="B537" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="538" spans="1:2">
+      <c r="A538" s="1">
+        <v>536</v>
+      </c>
+      <c r="B538" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="539" spans="1:2">
+      <c r="A539" s="1">
+        <v>537</v>
+      </c>
+      <c r="B539" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="540" spans="1:2">
+      <c r="A540" s="1">
+        <v>538</v>
+      </c>
+      <c r="B540" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="541" spans="1:2">
+      <c r="A541" s="1">
+        <v>539</v>
+      </c>
+      <c r="B541" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Got auto tempo feature running! Now works with any/most chordify links
</commit_message>
<xml_diff>
--- a/chords.xlsx
+++ b/chords.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B287"/>
+  <dimension ref="A1:B423"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -379,7 +379,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>rest</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -389,7 +389,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>rest</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -399,7 +399,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>rest</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -409,7 +409,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>rest</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -459,7 +459,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
     </row>
@@ -469,7 +469,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
     </row>
@@ -479,7 +479,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
     </row>
@@ -489,7 +489,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
     </row>
@@ -539,7 +539,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>rest</t>
         </is>
       </c>
     </row>
@@ -549,7 +549,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>rest</t>
         </is>
       </c>
     </row>
@@ -559,7 +559,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>rest</t>
         </is>
       </c>
     </row>
@@ -569,7 +569,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>rest</t>
         </is>
       </c>
     </row>
@@ -579,7 +579,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>rest</t>
         </is>
       </c>
     </row>
@@ -589,7 +589,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>rest</t>
         </is>
       </c>
     </row>
@@ -599,7 +599,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>rest</t>
         </is>
       </c>
     </row>
@@ -609,7 +609,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>rest</t>
         </is>
       </c>
     </row>
@@ -619,7 +619,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>rest</t>
         </is>
       </c>
     </row>
@@ -629,7 +629,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>rest</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -669,7 +669,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -679,7 +679,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -689,7 +689,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -699,7 +699,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>rest</t>
         </is>
       </c>
     </row>
@@ -709,7 +709,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>rest</t>
         </is>
       </c>
     </row>
@@ -719,7 +719,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>rest</t>
         </is>
       </c>
     </row>
@@ -729,7 +729,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>rest</t>
         </is>
       </c>
     </row>
@@ -739,7 +739,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>rest</t>
         </is>
       </c>
     </row>
@@ -749,7 +749,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>rest</t>
         </is>
       </c>
     </row>
@@ -759,7 +759,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>rest</t>
         </is>
       </c>
     </row>
@@ -769,7 +769,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>rest</t>
         </is>
       </c>
     </row>
@@ -779,7 +779,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>F#m7</t>
         </is>
       </c>
     </row>
@@ -789,7 +789,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>F#m7</t>
         </is>
       </c>
     </row>
@@ -799,7 +799,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>F#m7</t>
         </is>
       </c>
     </row>
@@ -809,7 +809,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>F#m7</t>
         </is>
       </c>
     </row>
@@ -819,7 +819,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>F#m7</t>
         </is>
       </c>
     </row>
@@ -829,7 +829,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>F#m7</t>
         </is>
       </c>
     </row>
@@ -839,7 +839,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>F#m7</t>
         </is>
       </c>
     </row>
@@ -849,7 +849,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>F#</t>
         </is>
       </c>
     </row>
@@ -859,7 +859,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>E7</t>
         </is>
       </c>
     </row>
@@ -869,7 +869,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>E7</t>
         </is>
       </c>
     </row>
@@ -879,7 +879,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>E7</t>
         </is>
       </c>
     </row>
@@ -889,7 +889,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>E7</t>
         </is>
       </c>
     </row>
@@ -899,7 +899,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -909,7 +909,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -919,7 +919,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -929,7 +929,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -939,7 +939,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -949,7 +949,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -959,7 +959,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C#m</t>
         </is>
       </c>
     </row>
@@ -969,7 +969,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C#m</t>
         </is>
       </c>
     </row>
@@ -979,7 +979,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>F#</t>
         </is>
       </c>
     </row>
@@ -989,7 +989,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>F#</t>
         </is>
       </c>
     </row>
@@ -999,7 +999,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>F#</t>
         </is>
       </c>
     </row>
@@ -1009,7 +1009,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>F#</t>
         </is>
       </c>
     </row>
@@ -1019,7 +1019,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -1029,7 +1029,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -1039,7 +1039,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -1049,7 +1049,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -1059,7 +1059,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>B</t>
         </is>
       </c>
     </row>
@@ -1069,7 +1069,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>B</t>
         </is>
       </c>
     </row>
@@ -1079,7 +1079,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>B</t>
         </is>
       </c>
     </row>
@@ -1089,7 +1089,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>B</t>
         </is>
       </c>
     </row>
@@ -1099,7 +1099,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -1109,7 +1109,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -1119,7 +1119,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -1129,7 +1129,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -1139,7 +1139,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -1149,7 +1149,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -1159,7 +1159,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -1169,7 +1169,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -1179,7 +1179,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -1189,7 +1189,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -1199,7 +1199,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -1259,7 +1259,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -1269,7 +1269,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -1279,7 +1279,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -1289,7 +1289,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -1299,7 +1299,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>F#</t>
         </is>
       </c>
     </row>
@@ -1309,7 +1309,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>F#</t>
         </is>
       </c>
     </row>
@@ -1319,7 +1319,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>F#</t>
         </is>
       </c>
     </row>
@@ -1329,7 +1329,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>F#</t>
         </is>
       </c>
     </row>
@@ -1339,7 +1339,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>F#</t>
         </is>
       </c>
     </row>
@@ -1349,7 +1349,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>F#</t>
         </is>
       </c>
     </row>
@@ -1359,7 +1359,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -1369,7 +1369,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -1379,7 +1379,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -1389,7 +1389,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -1399,7 +1399,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>B</t>
         </is>
       </c>
     </row>
@@ -1409,7 +1409,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>B</t>
         </is>
       </c>
     </row>
@@ -1419,7 +1419,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
     </row>
@@ -1429,7 +1429,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
     </row>
@@ -1439,7 +1439,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
     </row>
@@ -1449,7 +1449,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
     </row>
@@ -1459,7 +1459,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -1469,7 +1469,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -1479,7 +1479,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -1489,7 +1489,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -1499,7 +1499,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -1509,7 +1509,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -1539,7 +1539,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -1549,7 +1549,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -1579,7 +1579,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -1589,7 +1589,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -1599,7 +1599,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C#m</t>
         </is>
       </c>
     </row>
@@ -1609,7 +1609,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C#m</t>
         </is>
       </c>
     </row>
@@ -1619,7 +1619,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -1629,7 +1629,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -1659,7 +1659,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -1669,7 +1669,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -1679,7 +1679,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -1689,7 +1689,7 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -1699,7 +1699,7 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>B</t>
         </is>
       </c>
     </row>
@@ -1709,7 +1709,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>B</t>
         </is>
       </c>
     </row>
@@ -1739,7 +1739,7 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -1749,7 +1749,7 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -1759,7 +1759,7 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>F#</t>
         </is>
       </c>
     </row>
@@ -1769,7 +1769,7 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>F#</t>
         </is>
       </c>
     </row>
@@ -1779,7 +1779,7 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -1789,7 +1789,7 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -1809,7 +1809,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -1819,7 +1819,7 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -1829,7 +1829,7 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -1839,7 +1839,7 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -1849,7 +1849,7 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -1879,7 +1879,7 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -1889,7 +1889,7 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -1939,7 +1939,7 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -1949,7 +1949,7 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -1959,7 +1959,7 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -1969,7 +1969,7 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -1979,7 +1979,7 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -1989,7 +1989,7 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -1999,7 +1999,7 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -2009,7 +2009,7 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -2019,7 +2019,7 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -2029,7 +2029,7 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -2059,7 +2059,7 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
     </row>
@@ -2069,7 +2069,7 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
     </row>
@@ -2079,7 +2079,7 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
     </row>
@@ -2089,7 +2089,7 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
     </row>
@@ -2099,7 +2099,7 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>B</t>
         </is>
       </c>
     </row>
@@ -2109,7 +2109,7 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>B</t>
         </is>
       </c>
     </row>
@@ -2119,7 +2119,7 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -2129,7 +2129,7 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -2139,7 +2139,7 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -2149,7 +2149,7 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -2159,7 +2159,7 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -2169,7 +2169,7 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -2189,7 +2189,7 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>Em</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -2199,7 +2199,7 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>Em</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -2209,7 +2209,7 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>Em</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -2219,7 +2219,7 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -2229,7 +2229,7 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -2239,7 +2239,7 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -2249,7 +2249,7 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -2259,7 +2259,7 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>Em</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -2269,7 +2269,7 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>Em</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -2279,7 +2279,7 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -2289,7 +2289,7 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -2299,7 +2299,7 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -2309,7 +2309,7 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -2319,7 +2319,7 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -2329,7 +2329,7 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -2339,7 +2339,7 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -2349,7 +2349,7 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>B</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>B</t>
         </is>
       </c>
     </row>
@@ -2379,7 +2379,7 @@
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -2389,7 +2389,7 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -2399,7 +2399,7 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -2409,7 +2409,7 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -2419,7 +2419,7 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -2429,7 +2429,7 @@
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -2439,7 +2439,7 @@
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>C#m</t>
         </is>
       </c>
     </row>
@@ -2449,7 +2449,7 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>C#m</t>
         </is>
       </c>
     </row>
@@ -2459,7 +2459,7 @@
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -2469,7 +2469,7 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -2479,7 +2479,7 @@
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -2489,7 +2489,7 @@
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -2499,7 +2499,7 @@
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D7</t>
         </is>
       </c>
     </row>
@@ -2509,7 +2509,7 @@
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D7</t>
         </is>
       </c>
     </row>
@@ -2519,7 +2519,7 @@
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D7</t>
         </is>
       </c>
     </row>
@@ -2529,7 +2529,7 @@
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D7</t>
         </is>
       </c>
     </row>
@@ -2539,7 +2539,7 @@
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -2549,7 +2549,7 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -2579,7 +2579,7 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -2589,7 +2589,7 @@
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -2599,7 +2599,7 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>C#m</t>
         </is>
       </c>
     </row>
@@ -2609,7 +2609,7 @@
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>C#m</t>
         </is>
       </c>
     </row>
@@ -2619,7 +2619,7 @@
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C#m7</t>
         </is>
       </c>
     </row>
@@ -2629,7 +2629,7 @@
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C#m7</t>
         </is>
       </c>
     </row>
@@ -2639,7 +2639,7 @@
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -2649,7 +2649,7 @@
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -2659,7 +2659,7 @@
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -2669,7 +2669,7 @@
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -2679,7 +2679,7 @@
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -2689,7 +2689,7 @@
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -2699,7 +2699,7 @@
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
     </row>
@@ -2709,7 +2709,7 @@
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
     </row>
@@ -2719,7 +2719,7 @@
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
     </row>
@@ -2729,7 +2729,7 @@
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
     </row>
@@ -2739,7 +2739,7 @@
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -2749,7 +2749,7 @@
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -2759,7 +2759,7 @@
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -2769,7 +2769,7 @@
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -2779,7 +2779,7 @@
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -2789,7 +2789,7 @@
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -2799,7 +2799,7 @@
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -2809,7 +2809,7 @@
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -2819,7 +2819,7 @@
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -2829,7 +2829,7 @@
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -2839,7 +2839,7 @@
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -2849,7 +2849,7 @@
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -2859,7 +2859,7 @@
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -2869,7 +2869,7 @@
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C#m</t>
         </is>
       </c>
     </row>
@@ -2879,7 +2879,7 @@
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>C#m</t>
         </is>
       </c>
     </row>
@@ -2889,7 +2889,7 @@
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>C#m</t>
         </is>
       </c>
     </row>
@@ -2899,7 +2899,7 @@
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>C#m</t>
         </is>
       </c>
     </row>
@@ -2909,7 +2909,7 @@
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -2919,7 +2919,7 @@
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -2929,7 +2929,7 @@
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -2939,7 +2939,7 @@
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -2949,7 +2949,7 @@
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -2959,7 +2959,7 @@
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>rest</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -2969,7 +2969,7 @@
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>rest</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -2979,7 +2979,7 @@
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>rest</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -2989,7 +2989,7 @@
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>rest</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -2999,7 +2999,7 @@
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>rest</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -3009,7 +3009,7 @@
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>rest</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -3019,7 +3019,7 @@
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>rest</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -3029,7 +3029,7 @@
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>rest</t>
+          <t>F#m</t>
         </is>
       </c>
     </row>
@@ -3039,7 +3039,7 @@
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>rest</t>
+          <t>C#m</t>
         </is>
       </c>
     </row>
@@ -3049,7 +3049,7 @@
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>rest</t>
+          <t>C#m</t>
         </is>
       </c>
     </row>
@@ -3059,7 +3059,7 @@
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>rest</t>
+          <t>C#m</t>
         </is>
       </c>
     </row>
@@ -3069,7 +3069,7 @@
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>rest</t>
+          <t>C#m</t>
         </is>
       </c>
     </row>
@@ -3079,7 +3079,7 @@
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>rest</t>
+          <t>C#m</t>
         </is>
       </c>
     </row>
@@ -3089,7 +3089,7 @@
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>rest</t>
+          <t>C#m</t>
         </is>
       </c>
     </row>
@@ -3099,7 +3099,7 @@
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>rest</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -3109,7 +3109,7 @@
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>rest</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -3119,7 +3119,7 @@
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>rest</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -3129,7 +3129,7 @@
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>rest</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -3139,7 +3139,7 @@
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>rest</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -3149,7 +3149,7 @@
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>rest</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -3159,7 +3159,7 @@
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>rest</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -3169,7 +3169,7 @@
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>rest</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -3179,7 +3179,7 @@
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>rest</t>
+          <t>C#</t>
         </is>
       </c>
     </row>
@@ -3189,7 +3189,7 @@
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>rest</t>
+          <t>C#</t>
         </is>
       </c>
     </row>
@@ -3199,7 +3199,7 @@
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>rest</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -3209,7 +3209,7 @@
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>rest</t>
+          <t>A</t>
         </is>
       </c>
     </row>
@@ -3219,7 +3219,7 @@
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>rest</t>
+          <t>E</t>
         </is>
       </c>
     </row>
@@ -3228,6 +3228,1366 @@
         <v>285</v>
       </c>
       <c r="B287" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" s="1" t="n">
+        <v>286</v>
+      </c>
+      <c r="B288" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" s="1" t="n">
+        <v>287</v>
+      </c>
+      <c r="B289" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" s="1" t="n">
+        <v>288</v>
+      </c>
+      <c r="B290" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" s="1" t="n">
+        <v>289</v>
+      </c>
+      <c r="B291" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" s="1" t="n">
+        <v>290</v>
+      </c>
+      <c r="B292" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" s="1" t="n">
+        <v>291</v>
+      </c>
+      <c r="B293" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" s="1" t="n">
+        <v>292</v>
+      </c>
+      <c r="B294" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" s="1" t="n">
+        <v>293</v>
+      </c>
+      <c r="B295" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" s="1" t="n">
+        <v>294</v>
+      </c>
+      <c r="B296" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" s="1" t="n">
+        <v>295</v>
+      </c>
+      <c r="B297" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" s="1" t="n">
+        <v>296</v>
+      </c>
+      <c r="B298" t="inlineStr">
+        <is>
+          <t>F#m7</t>
+        </is>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" s="1" t="n">
+        <v>297</v>
+      </c>
+      <c r="B299" t="inlineStr">
+        <is>
+          <t>F#m7</t>
+        </is>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" s="1" t="n">
+        <v>298</v>
+      </c>
+      <c r="B300" t="inlineStr">
+        <is>
+          <t>B7</t>
+        </is>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" s="1" t="n">
+        <v>299</v>
+      </c>
+      <c r="B301" t="inlineStr">
+        <is>
+          <t>B7</t>
+        </is>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" s="1" t="n">
+        <v>300</v>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" s="1" t="n">
+        <v>301</v>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" s="1" t="n">
+        <v>302</v>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" s="1" t="n">
+        <v>303</v>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" s="1" t="n">
+        <v>304</v>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" s="1" t="n">
+        <v>305</v>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" s="1" t="n">
+        <v>306</v>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" s="1" t="n">
+        <v>307</v>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" s="1" t="n">
+        <v>308</v>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" s="1" t="n">
+        <v>309</v>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" s="1" t="n">
+        <v>310</v>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" s="1" t="n">
+        <v>311</v>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" s="1" t="n">
+        <v>312</v>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>C#</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" s="1" t="n">
+        <v>313</v>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>C#</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" s="1" t="n">
+        <v>314</v>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" s="1" t="n">
+        <v>315</v>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" s="1" t="n">
+        <v>316</v>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" s="1" t="n">
+        <v>317</v>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" s="1" t="n">
+        <v>318</v>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" s="1" t="n">
+        <v>319</v>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" s="1" t="n">
+        <v>320</v>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" s="1" t="n">
+        <v>321</v>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" s="1" t="n">
+        <v>322</v>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" s="1" t="n">
+        <v>323</v>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" s="1" t="n">
+        <v>324</v>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" s="1" t="n">
+        <v>325</v>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" s="1" t="n">
+        <v>326</v>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" s="1" t="n">
+        <v>327</v>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" s="1" t="n">
+        <v>328</v>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>F#m</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" s="1" t="n">
+        <v>329</v>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>F#m</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" s="1" t="n">
+        <v>330</v>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" s="1" t="n">
+        <v>331</v>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" s="1" t="n">
+        <v>332</v>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" s="1" t="n">
+        <v>333</v>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" s="1" t="n">
+        <v>334</v>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" s="1" t="n">
+        <v>335</v>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" s="1" t="n">
+        <v>336</v>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>F#m</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" s="1" t="n">
+        <v>337</v>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>F#m</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" s="1" t="n">
+        <v>338</v>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" s="1" t="n">
+        <v>339</v>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" s="1" t="n">
+        <v>340</v>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" s="1" t="n">
+        <v>341</v>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" s="1" t="n">
+        <v>342</v>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" s="1" t="n">
+        <v>343</v>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" s="1" t="n">
+        <v>344</v>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" s="1" t="n">
+        <v>345</v>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>F#m7</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" s="1" t="n">
+        <v>346</v>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>F#m7</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" s="1" t="n">
+        <v>347</v>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>F#m7</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" s="1" t="n">
+        <v>348</v>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>B7</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" s="1" t="n">
+        <v>349</v>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>B7</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" s="1" t="n">
+        <v>350</v>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>B7</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" s="1" t="n">
+        <v>351</v>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>B7</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" s="1" t="n">
+        <v>352</v>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>B7</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" s="1" t="n">
+        <v>353</v>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>B7</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" s="1" t="n">
+        <v>354</v>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>B7</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" s="1" t="n">
+        <v>355</v>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>B7</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" s="1" t="n">
+        <v>356</v>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" s="1" t="n">
+        <v>357</v>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" s="1" t="n">
+        <v>358</v>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" s="1" t="n">
+        <v>359</v>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" s="1" t="n">
+        <v>360</v>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" s="1" t="n">
+        <v>361</v>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" s="1" t="n">
+        <v>362</v>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" s="1" t="n">
+        <v>363</v>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" s="1" t="n">
+        <v>364</v>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" s="1" t="n">
+        <v>365</v>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" s="1" t="n">
+        <v>366</v>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" s="1" t="n">
+        <v>367</v>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" s="1" t="n">
+        <v>368</v>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" s="1" t="n">
+        <v>369</v>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" s="1" t="n">
+        <v>370</v>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" s="1" t="n">
+        <v>371</v>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" s="1" t="n">
+        <v>372</v>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>rest</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" s="1" t="n">
+        <v>373</v>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>rest</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" s="1" t="n">
+        <v>374</v>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>rest</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" s="1" t="n">
+        <v>375</v>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>rest</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" s="1" t="n">
+        <v>376</v>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>rest</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" s="1" t="n">
+        <v>377</v>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>rest</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" s="1" t="n">
+        <v>378</v>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>rest</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" s="1" t="n">
+        <v>379</v>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>rest</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" s="1" t="n">
+        <v>380</v>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>rest</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" s="1" t="n">
+        <v>381</v>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>rest</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" s="1" t="n">
+        <v>382</v>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>rest</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" s="1" t="n">
+        <v>383</v>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>rest</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" s="1" t="n">
+        <v>384</v>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>rest</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" s="1" t="n">
+        <v>385</v>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>rest</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" s="1" t="n">
+        <v>386</v>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>rest</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" s="1" t="n">
+        <v>387</v>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>rest</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" s="1" t="n">
+        <v>388</v>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>rest</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" s="1" t="n">
+        <v>389</v>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>rest</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" s="1" t="n">
+        <v>390</v>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>rest</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" s="1" t="n">
+        <v>391</v>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>rest</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" s="1" t="n">
+        <v>392</v>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>rest</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" s="1" t="n">
+        <v>393</v>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>rest</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" s="1" t="n">
+        <v>394</v>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>rest</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" s="1" t="n">
+        <v>395</v>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>rest</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" s="1" t="n">
+        <v>396</v>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>rest</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" s="1" t="n">
+        <v>397</v>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>rest</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" s="1" t="n">
+        <v>398</v>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>rest</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" s="1" t="n">
+        <v>399</v>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>rest</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" s="1" t="n">
+        <v>400</v>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>rest</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" s="1" t="n">
+        <v>401</v>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>rest</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" s="1" t="n">
+        <v>402</v>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>rest</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" s="1" t="n">
+        <v>403</v>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>rest</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" s="1" t="n">
+        <v>404</v>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>rest</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" s="1" t="n">
+        <v>405</v>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>rest</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" s="1" t="n">
+        <v>406</v>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>rest</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" s="1" t="n">
+        <v>407</v>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>rest</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" s="1" t="n">
+        <v>408</v>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>rest</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" s="1" t="n">
+        <v>409</v>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>rest</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" s="1" t="n">
+        <v>410</v>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>rest</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" s="1" t="n">
+        <v>411</v>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>rest</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" s="1" t="n">
+        <v>412</v>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>rest</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" s="1" t="n">
+        <v>413</v>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>rest</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" s="1" t="n">
+        <v>414</v>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>rest</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" s="1" t="n">
+        <v>415</v>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>rest</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" s="1" t="n">
+        <v>416</v>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>rest</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" s="1" t="n">
+        <v>417</v>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>rest</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" s="1" t="n">
+        <v>418</v>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>rest</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" s="1" t="n">
+        <v>419</v>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>rest</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" s="1" t="n">
+        <v>420</v>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>rest</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" s="1" t="n">
+        <v>421</v>
+      </c>
+      <c r="B423" t="inlineStr">
         <is>
           <t>rest</t>
         </is>

</xml_diff>